<commit_message>
added frameworks and licenses
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64ABE908-81C4-4594-B66C-BAAD192AAF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EDBB75-36F5-4ECA-B1E8-FF36E763481B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="License" sheetId="3" r:id="rId2"/>
+    <sheet name="Revisions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +37,137 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+  <si>
+    <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
+  </si>
+  <si>
+    <t>1. Redistributions of source code must retain the above copyright notice, this list of conditions and the following disclaimer.</t>
+  </si>
+  <si>
+    <t>2. Redistributions in binary form must reproduce the above copyright notice, this list of conditions and the following disclaimer in the documentation and/or other materials provided with the distribution.</t>
+  </si>
+  <si>
+    <t>3. Neither the name of the copyright holder nor the names of its contributors may be used to endorse or promote products derived from this software without specific prior written permission.</t>
+  </si>
+  <si>
+    <t>THIS SOFTWARE IS PROVIDED BY THE COPYRIGHT HOLDERS AND CONTRIBUTORS “AS IS” AND ANY EXPRESS OR IMPLIED WARRANTIES, INCLUDING, BUT NOT LIMITED TO, THE IMPLIED WARRANTIES OF MERCHANTABILITY AND FITNESS FOR A PARTICULAR PURPOSE ARE DISCLAIMED. IN NO EVENT SHALL THE COPYRIGHT HOLDER OR CONTRIBUTORS BE LIABLE FOR ANY DIRECT, INDIRECT, INCIDENTAL, SPECIAL, EXEMPLARY, OR CONSEQUENTIAL DAMAGES (INCLUDING, BUT NOT LIMITED TO, PROCUREMENT OF SUBSTITUTE GOODS OR SERVICES; LOSS OF USE, DATA, OR PROFITS; OR BUSINESS INTERRUPTION) HOWEVER CAUSED AND ON ANY THEORY OF LIABILITY, WHETHER IN CONTRACT, STRICT LIABILITY, OR TORT (INCLUDING NEGLIGENCE OR OTHERWISE) ARISING IN ANY WAY OUT OF THE USE OF THIS SOFTWARE, EVEN IF ADVISED OF THE POSSIBILITY OF SUCH DAMAGE.</t>
+  </si>
+  <si>
+    <t>Copyright 2023 Erik Wilhelm</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Author(s)</t>
+  </si>
+  <si>
+    <t>Initial commit</t>
+  </si>
+  <si>
+    <t>Changelog</t>
+  </si>
+  <si>
+    <t>added licence and overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated Ground Vehicle Use Case Model </t>
+  </si>
+  <si>
+    <t>The overarching goal of the model is to enable the economic feasibility of a wide variety of autonomous ground vehicle projects to be objectively evaluated. To achieve this goal, the model aims to answer the following questions:</t>
+  </si>
+  <si>
+    <t>1. What is the net present value of an investment in an automated ground vehicle for a specific application use case compared to the business as usual case?</t>
+  </si>
+  <si>
+    <t>2. What is the sensitivity of the amortization period to the input assumptions? In other words, which input assumptions have the greatest effect on the amortization period for the project?</t>
+  </si>
+  <si>
+    <t>3. Which implications do the deployment of automated ground robots have on manpower needs? In other words, where can human resources be more effectively allocated?</t>
+  </si>
+  <si>
+    <t>Contributors</t>
+  </si>
+  <si>
+    <t>Erik Wilhelm</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Kyburz Switzerland</t>
+  </si>
+  <si>
+    <t>Christoph Kammer</t>
+  </si>
+  <si>
+    <t>The Mathworks</t>
+  </si>
+  <si>
+    <t>Flurin Arner</t>
+  </si>
+  <si>
+    <t>Flurin Arner Inc</t>
+  </si>
+  <si>
+    <t>Markus Rohr</t>
+  </si>
+  <si>
+    <t>Robolem</t>
+  </si>
+  <si>
+    <t>AMAG</t>
+  </si>
+  <si>
+    <t>ETH Zürich</t>
+  </si>
+  <si>
+    <t>Christoph Zeier</t>
+  </si>
+  <si>
+    <t>Cyril Zubr</t>
+  </si>
+  <si>
+    <t>The inputs, outputs, and assumptions of the model are outlined in their respective worksheets.</t>
+  </si>
+  <si>
+    <t>Please see the licence worksheet before deploying this model.</t>
+  </si>
+  <si>
+    <t>If you use this model, please use this citation:</t>
+  </si>
+  <si>
+    <t>Please see this paper for details about the assumptions, inputs, and for worked examples.</t>
+  </si>
+  <si>
+    <t>LINK TO PAPER</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>11.Aug.2023</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +191,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +529,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1454754-4F99-4FD9-969E-48E849408383}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28220BA-D6B8-4BF3-9DEF-B47EF2B32EFA}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE02DBDA-DE44-4252-90B2-55A50E3DF62B}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
functionalized use case calculation model for running sensitivity
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EDBB75-36F5-4ECA-B1E8-FF36E763481B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F10E0F9-2660-4DEA-A696-0CCEB944643C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="29400" yWindow="1770" windowWidth="26430" windowHeight="13890" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="License" sheetId="3" r:id="rId2"/>
     <sheet name="Revisions" sheetId="2" r:id="rId3"/>
+    <sheet name="Assumptions" sheetId="4" r:id="rId4"/>
+    <sheet name="Inputs" sheetId="5" r:id="rId5"/>
+    <sheet name="Outputs" sheetId="6" r:id="rId6"/>
+    <sheet name="Sensitivity" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -531,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1454754-4F99-4FD9-969E-48E849408383}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE02DBDA-DE44-4252-90B2-55A50E3DF62B}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -912,4 +916,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D618CA9B-8483-4F01-824C-AFC919087770}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CCFE16-9466-4B3B-9B84-9ACED9823E1B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3921CD35-E3FB-4076-863C-CDE02BDE2C9B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E08E8B2-3823-4F4D-943E-C68B1F535EDC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added structure for modeling AGV mission and mission assumption to excel
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F10E0F9-2660-4DEA-A696-0CCEB944643C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA1EDB-37DF-44AA-A188-F9952EA2D0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="1770" windowWidth="26430" windowHeight="13890" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="29850" yWindow="660" windowWidth="27165" windowHeight="15540" activeTab="7" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Inputs" sheetId="5" r:id="rId5"/>
     <sheet name="Outputs" sheetId="6" r:id="rId6"/>
     <sheet name="Sensitivity" sheetId="7" r:id="rId7"/>
+    <sheet name="TechMaturity" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -156,13 +157,106 @@
   </si>
   <si>
     <t>11.Aug.2023</t>
+  </si>
+  <si>
+    <t>TRL</t>
+  </si>
+  <si>
+    <t>Basic principles observed and reported</t>
+  </si>
+  <si>
+    <t>Basic principles observed</t>
+  </si>
+  <si>
+    <t>Technology concept and/or application formulated</t>
+  </si>
+  <si>
+    <t>Technology concept formulated</t>
+  </si>
+  <si>
+    <t>Analytical and experimental critical function and/or characteristic proof-of concept</t>
+  </si>
+  <si>
+    <t>Experimental proof of concept</t>
+  </si>
+  <si>
+    <t>Component and/or breadboard validation in laboratory environment</t>
+  </si>
+  <si>
+    <t>Technology validated in lab</t>
+  </si>
+  <si>
+    <t>Component and/or breadboard validation in relevant environment</t>
+  </si>
+  <si>
+    <t>Technology validated in relevant environment (industrially relevant environment in the case of key enabling technologies)</t>
+  </si>
+  <si>
+    <t>System/subsystem model or prototype demonstration in a relevant environment (ground or space)</t>
+  </si>
+  <si>
+    <t>Technology demonstrated in relevant environment (industrially relevant environment in the case of key enabling technologies)</t>
+  </si>
+  <si>
+    <t>System prototype demonstration in a space environment</t>
+  </si>
+  <si>
+    <t>System prototype demonstration in operational environment</t>
+  </si>
+  <si>
+    <t>Actual system completed and "flight qualified" through test and demonstration (ground or space)</t>
+  </si>
+  <si>
+    <t>System complete and qualified</t>
+  </si>
+  <si>
+    <t>Actual system "flight proven" through successful mission operations</t>
+  </si>
+  <si>
+    <t>Actual system proven in operational environment (competitive manufacturing in the case of key enabling technologies; or in space)</t>
+  </si>
+  <si>
+    <t>NASA usage</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Technology_readiness_level</t>
+  </si>
+  <si>
+    <t>Number of Vehicles Deployed</t>
+  </si>
+  <si>
+    <t>Number of Hours Operated</t>
+  </si>
+  <si>
+    <t>Approx. Company Size</t>
+  </si>
+  <si>
+    <t>3000+</t>
+  </si>
+  <si>
+    <t>Years of Experience</t>
+  </si>
+  <si>
+    <t>disengagement per km</t>
+  </si>
+  <si>
+    <t>km between disengagement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +268,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,16 +313,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -234,6 +345,1098 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Disengagement per km</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TechMaturity!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>disengagement per km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000">
+                  <c:v>3.3333333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000">
+                  <c:v>1.6666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000">
+                  <c:v>1.1111111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000">
+                  <c:v>8.3333333333333339E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="844849416"/>
+        <c:axId val="844850496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="844849416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Technology</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Readiness Level</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844850496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="844850496"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Disengagements/km</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844849416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>747711</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75FAEFB5-CF97-808B-044C-922CD0CA7B77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,7 +1738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1454754-4F99-4FD9-969E-48E849408383}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
@@ -546,7 +1749,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -571,10 +1774,10 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -719,199 +1922,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>0.1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -964,4 +2167,347 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52113A14-9B74-4A0A-A854-9B7F98F5B3B4}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>D2*212*8.25*7</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <f>1/H2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">D3*212*8.25*7</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="1">1/H3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>12243</v>
+      </c>
+      <c r="F6">
+        <v>150</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>150</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666671E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>12243</v>
+      </c>
+      <c r="F7">
+        <v>300</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>300</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>122430</v>
+      </c>
+      <c r="F8">
+        <v>900</v>
+      </c>
+      <c r="G8">
+        <v>40</v>
+      </c>
+      <c r="H8">
+        <v>600</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666668E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1224300</v>
+      </c>
+      <c r="F9">
+        <v>1500</v>
+      </c>
+      <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="H9">
+        <v>900</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>1.1111111111111111E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>12243000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>1200</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{4D0C079C-674A-4326-B620-BADC61C3A795}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added to the technology readiness sensitivity - not yet complete
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA1EDB-37DF-44AA-A188-F9952EA2D0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E813C9-9FC1-4AE8-95F5-D7802A1DD596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29850" yWindow="660" windowWidth="27165" windowHeight="15540" activeTab="7" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="Outputs" sheetId="6" r:id="rId6"/>
     <sheet name="Sensitivity" sheetId="7" r:id="rId7"/>
     <sheet name="TechMaturity" sheetId="8" r:id="rId8"/>
+    <sheet name="MissionComplexity" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -247,14 +248,27 @@
   </si>
   <si>
     <t>km between disengagement</t>
+  </si>
+  <si>
+    <t>min per disengagement</t>
+  </si>
+  <si>
+    <t>max_speed</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -317,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,7 +342,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -395,6 +410,556 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TechMaturity!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>disengagement per km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>3.3333333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>1.6666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>1.1111111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>8.3333333333333339E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TechMaturity!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>disengagement per km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.0253681195074532E-3"/>
+                  <c:y val="-0.19308852331403412"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>3.3333333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>1.6666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>1.1111111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>8.3333333333333339E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="844849416"/>
+        <c:axId val="844850496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="844849416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Technology</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Readiness Level</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844850496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="844850496"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Disengagements/km (LOG scale)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844849416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Minutes per Disengagement</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
       <c:txPr>
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
@@ -427,11 +992,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TechMaturity!$I$1</c:f>
+              <c:f>TechMaturity!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>disengagement per km</c:v>
+                  <c:v>min per disengagement</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -460,6 +1025,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.0253681195074532E-3"/>
+                  <c:y val="-0.19308852331403412"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>TechMaturity!$A$2:$A$10</c:f>
@@ -498,36 +1113,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:f>TechMaturity!$J$2:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.000">
-                  <c:v>6.6666666666666671E-3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.000">
-                  <c:v>3.3333333333333335E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.000">
-                  <c:v>1.6666666666666668E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.000">
-                  <c:v>1.1111111111111111E-3</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.000">
-                  <c:v>8.3333333333333339E-4</c:v>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,7 +1150,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+              <c16:uniqueId val="{00000001-CB9A-4417-80F6-B50A17412530}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -715,8 +1330,20 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Disengagements/km</a:t>
+                  <a:t>min/Disengagement </a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(LOG scale)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -751,7 +1378,564 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844849416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Max Speed </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TechMaturity!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max_speed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.159180405440194E-2"/>
+                  <c:y val="1.5207121645511183E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TechMaturity!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AE7D-4093-82C3-3580A4C85609}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="844849416"/>
+        <c:axId val="844850496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="844849416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Technology</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Readiness Level</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844850496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="844850496"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>max speed km/hr </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(LOG scale)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -882,6 +2066,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1398,20 +2622,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>557212</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>747711</xdr:rowOff>
+      <xdr:rowOff>357186</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>266699</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1431,6 +3171,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>342900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>481013</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC8CE692-13CA-42A4-9C1C-51FECF99A377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>242888</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>214313</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F89DD2-480B-4C6A-A8F9-FA2A822A78B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2171,10 +3987,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52113A14-9B74-4A0A-A854-9B7F98F5B3B4}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +4003,7 @@
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -2215,8 +4031,14 @@
       <c r="I1" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2242,12 +4064,18 @@
       <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="7">
         <f>1/H2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>120</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2273,12 +4101,18 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="7">
         <f t="shared" ref="I3:I11" si="1">1/H3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2304,12 +4138,18 @@
       <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="7">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2335,12 +4175,18 @@
       <c r="H5">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2370,8 +4216,14 @@
         <f t="shared" si="1"/>
         <v>6.6666666666666671E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2401,8 +4253,14 @@
         <f t="shared" si="1"/>
         <v>3.3333333333333335E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2432,8 +4290,14 @@
         <f t="shared" si="1"/>
         <v>1.6666666666666668E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2463,8 +4327,14 @@
         <f t="shared" si="1"/>
         <v>1.1111111111111111E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2494,13 +4364,27 @@
         <f t="shared" si="1"/>
         <v>8.3333333333333339E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0.5</v>
+      </c>
+      <c r="K10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2510,4 +4394,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52350377-D0B0-4FB7-AB26-7414C6CA7A19}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rearranged variables to follow flow, added mission modeling scale to excel
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E813C9-9FC1-4AE8-95F5-D7802A1DD596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695FAF98-4D19-41DD-9B00-907416400A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29850" yWindow="660" windowWidth="27165" windowHeight="15540" activeTab="7" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="29805" yWindow="540" windowWidth="27165" windowHeight="15540" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Outputs" sheetId="6" r:id="rId6"/>
     <sheet name="Sensitivity" sheetId="7" r:id="rId7"/>
     <sheet name="TechMaturity" sheetId="8" r:id="rId8"/>
-    <sheet name="MissionComplexity" sheetId="9" r:id="rId9"/>
+    <sheet name="MissionModel" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="117">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -259,7 +259,142 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t xml:space="preserve">This section </t>
+    <t>The basic maturity assumptions on the master branch in this section are used in the code cases.</t>
+  </si>
+  <si>
+    <t>Company acceptance</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>MissionSimilarity</t>
+  </si>
+  <si>
+    <t>Example(s)</t>
+  </si>
+  <si>
+    <t>MissionDeterminism</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Some</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Sufficient</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outstanding </t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Company A takes over Company B's production process, inheriting proof-of-concept stage AGV systems in the aquisition; neither managment nor operations tolerates the pilot systems</t>
+  </si>
+  <si>
+    <t>Upper management forces production and logistics departments to trial new AGV technology for external marketing purposes</t>
+  </si>
+  <si>
+    <t>Well meaning senior department heads procure AGVs without adequate consultation of logistics needs; systems are viewed as too expensive and slow</t>
+  </si>
+  <si>
+    <t>AGV system was procured with cross-management agreement, but before delivery company priorities and processes changed; system no longer serves present needs</t>
+  </si>
+  <si>
+    <t>older generation AGV in service for several years, value in process is hard to justify; logistics and production tolerate system presense</t>
+  </si>
+  <si>
+    <t>value of AGV is clear to articulate in ist application; and is understood by management and supervisors</t>
+  </si>
+  <si>
+    <t>AGV works well in its mission, and its value is understood by all employees, including those sharing the shop floor with the system</t>
+  </si>
+  <si>
+    <t>AGV supports the employees in mission-critical ways, and is valued highly at all levels</t>
+  </si>
+  <si>
+    <t>AGV is viewed as critical for the success of the process to which its mission contributes</t>
+  </si>
+  <si>
+    <t>Without the AGV, the system process is viewed as being impossible</t>
+  </si>
+  <si>
+    <t>Each mission is completely different from the next</t>
+  </si>
+  <si>
+    <t>There are some similarites between missions (e.g. they all start and end with a charging step)</t>
+  </si>
+  <si>
+    <t>Parts of the mission are common between missions (e.g. the last building is always the same)</t>
+  </si>
+  <si>
+    <t>The start and end buildings are the same, but the route is vastly different</t>
+  </si>
+  <si>
+    <t>Only a few options exist for the robot to complete its mission; these can only be modified by trained employees</t>
+  </si>
+  <si>
+    <t>There are many pre-programmed routes which are followed by the AGVs, but they are free to choose a route as desired; new routes trained by anyone</t>
+  </si>
+  <si>
+    <t>Two options exist for the robot to complete its mission; these can only be programmed by AGV manufacturer</t>
+  </si>
+  <si>
+    <t>One route programmed by the AGV manufacture exits; it changes every quarter</t>
+  </si>
+  <si>
+    <t>One route programmed by the AGV manufacture exits; it changes every year</t>
+  </si>
+  <si>
+    <t>One route programmed by the AGV manufacture exits; it never changes</t>
+  </si>
+  <si>
+    <t>Peak periods of different vehicles and pedestrians (e.g. lunch time rush of bikes, cars, and people in front of a busy restaurant, but otherwise fewer obstacles)</t>
+  </si>
+  <si>
+    <t>Massive numbers of different types of vehicles and pedestrians (e.g. downtown manhattan at rush hour); this traffic persists throughout the day</t>
+  </si>
+  <si>
+    <t>Steady streams of moderate traffic</t>
+  </si>
+  <si>
+    <t>Periods of moderate traffic, but mostly open roads</t>
+  </si>
+  <si>
+    <t>Mostly open roads, periodic appearance of dynamic obstacles</t>
+  </si>
+  <si>
+    <t>Occasional dynamic obstacles, which are all aware of the AGV's presence and attention</t>
+  </si>
+  <si>
+    <t>Occasional dynamic obstacles, some of whom are untrained</t>
+  </si>
+  <si>
+    <t>Rare dynamic obstacles, which are all aware of the AGV's presence and attention</t>
+  </si>
+  <si>
+    <t>Open road, but no planned dynamic obstacles (e.g. possible to enter AGVs path if traffic rules on site are not followed)</t>
+  </si>
+  <si>
+    <t>Closed road, difficult for dynamic obstacles to enter the AGVs path, even if rules are not followed</t>
   </si>
 </sst>
 </file>
@@ -267,8 +402,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -342,8 +477,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3989,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52113A14-9B74-4A0A-A854-9B7F98F5B3B4}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I11" si="1">1/H3</f>
+        <f t="shared" ref="I3:I10" si="1">1/H3</f>
         <v>1</v>
       </c>
       <c r="J3">
@@ -4379,7 +4514,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -4398,12 +4533,376 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52350377-D0B0-4FB7-AB26-7414C6CA7A19}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="4" max="4" width="168" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8">
+        <v>0.6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9">
+        <v>0.7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11">
+        <v>0.9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18">
+        <v>0.4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>0.6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21">
+        <v>0.7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22">
+        <v>0.8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23">
+        <v>0.9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27">
+        <v>0.1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28">
+        <v>0.2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29">
+        <v>0.3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30">
+        <v>0.4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32">
+        <v>0.6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33">
+        <v>0.7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34">
+        <v>0.8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35">
+        <v>0.9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added additional comments, restructured for clarity
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695FAF98-4D19-41DD-9B00-907416400A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691332D8-91BF-45C3-A9EF-7B81CCAB908A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29805" yWindow="540" windowWidth="27165" windowHeight="15540" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="29805" yWindow="540" windowWidth="27165" windowHeight="15540" activeTab="7" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -4124,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52113A14-9B74-4A0A-A854-9B7F98F5B3B4}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4535,8 +4535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52350377-D0B0-4FB7-AB26-7414C6CA7A19}">
   <dimension ref="B2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
minor error correction in the script, added scenario outputs in excel, validated
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C31D8B-447B-470C-B820-D41A2AFF308A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4372B5-B10A-492D-900A-9412E8559F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="2" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="258">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -690,15 +690,171 @@
   </si>
   <si>
     <t>13.Dec.2023</t>
+  </si>
+  <si>
+    <t>Undiscounted lifetime costs</t>
+  </si>
+  <si>
+    <t>Human operated vehicle daily missions</t>
+  </si>
+  <si>
+    <t>Calculated inputs</t>
+  </si>
+  <si>
+    <t>missions/day</t>
+  </si>
+  <si>
+    <t>Human operated vehicle daily distance</t>
+  </si>
+  <si>
+    <t>km/day</t>
+  </si>
+  <si>
+    <t>Human operated vehicle daily driving time</t>
+  </si>
+  <si>
+    <t>vehicles</t>
+  </si>
+  <si>
+    <t>Human operated vehicle energy cost</t>
+  </si>
+  <si>
+    <t>Human operated vehicle operator cost</t>
+  </si>
+  <si>
+    <t>EUR/year</t>
+  </si>
+  <si>
+    <t>Human operated vehicle annual operating cost</t>
+  </si>
+  <si>
+    <t>Human operated vehicle annual maintenance cost</t>
+  </si>
+  <si>
+    <t>Human operated vehicle annual cost</t>
+  </si>
+  <si>
+    <t>Human operated vehicle end of life cost</t>
+  </si>
+  <si>
+    <t>Human operated vehicle purchase cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR </t>
+  </si>
+  <si>
+    <t>Human operated vehicle</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle daily missions</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle daily distance</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle daily driving time</t>
+  </si>
+  <si>
+    <t>Number of autonomous ground vehicles required</t>
+  </si>
+  <si>
+    <t>Number of human operated vehicles required</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle annual operating cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle energy cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle purchase cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle annual maintenance cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle annual cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle end of life cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle data cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle cost per disengagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autonomous ground vehicle disengagement </t>
+  </si>
+  <si>
+    <t>EUR/disengagement</t>
+  </si>
+  <si>
+    <t>Investment cost of switching to AGVs</t>
+  </si>
+  <si>
+    <t>Annual savings from switching to AGVs</t>
+  </si>
+  <si>
+    <t>End of life cost of switching to AGVs</t>
+  </si>
+  <si>
+    <t>Human operated vehice undiscounted lifetime cost</t>
+  </si>
+  <si>
+    <t>Autonomous ground vehicle undiscounted lifetime cost</t>
+  </si>
+  <si>
+    <t>Net present value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investement in AGV yields a net present value of </t>
+  </si>
+  <si>
+    <t>Cashflows</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Amortization period</t>
+  </si>
+  <si>
+    <t>Investement in AGV will pay back after</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>AGV</t>
+  </si>
+  <si>
+    <t>Cumulative annual vehicle operation cost</t>
+  </si>
+  <si>
+    <t>Cumulative annual autonomous vehicle operation cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -783,7 +939,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -801,6 +957,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -821,6 +982,1222 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> of Undiscounted Lifetime Costs</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Outputs!$D$37:$D$38</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Vehicle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AGV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Outputs!$B$37:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>150676.63400000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>142172.296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95DB-4414-AF15-D7B33B4828A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="790424216"/>
+        <c:axId val="790423496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="790424216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="790423496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="790423496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="790424216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Project Cash Flow</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Outputs!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Outputs!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Outputs!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-">
+                  <c:v>-41000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7386.3340000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7386.3340000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7386.3340000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7386.3340000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7386.3340000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7386.3340000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5186.3340000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9FFD-44E0-80D4-02C0E22996EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="865068784"/>
+        <c:axId val="865069144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="865068784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="865069144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="865069144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="865068784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Human operated vehicle lifetime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> cost share</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Outputs!$A$7,Outputs!$A$13:$A$14)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Human operated vehicle purchase cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cumulative annual vehicle operation cost</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Human operated vehicle end of life cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Outputs!$B$7,Outputs!$B$13:$B$14)</c:f>
+              <c:numCache>
+                <c:formatCode>_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>74000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74876.634000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D89-4BEB-8573-1B14763D2B2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Autonomous ground</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>vehicle lifetime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> cost share</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BDFE-4955-B7EF-34A0709E68CD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BDFE-4955-B7EF-34A0709E68CD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BDFE-4955-B7EF-34A0709E68CD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Outputs!$A$21,Outputs!$A$29:$A$30)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Autonomous ground vehicle purchase cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cumulative annual autonomous vehicle operation cost</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Autonomous ground vehicle end of life cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Outputs!$B$21,Outputs!$B$29:$B$30)</c:f>
+              <c:numCache>
+                <c:formatCode>_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23172.295999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BDFE-4955-B7EF-34A0709E68CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2151446735362601E-2"/>
+          <c:y val="0.77591326550372397"/>
+          <c:w val="0.88783856198122779"/>
+          <c:h val="0.1996964984007111"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -1370,7 +2747,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -1927,7 +3304,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -2564,8 +3941,168 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2592,8 +4129,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2694,7 +4231,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2726,10 +4263,1030 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3050,17 +5607,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3080,8 +5626,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3108,8 +5654,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3138,7 +5684,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -3189,6 +5735,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3199,18 +5752,25 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3245,7 +5805,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3566,6 +6126,511 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -3596,7 +6661,674 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3663758A-0EC9-56A0-7C94-42F7D6F0F42B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B8E0AB2-3DC2-D4BB-5DA2-57301BE49986}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC188DD1-373D-CBF0-B568-96A9846646EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E66DB761-4EFF-4FD1-98FE-B3DE239F8E62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5015,7 +8747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE02DBDA-DE44-4252-90B2-55A50E3DF62B}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5261,8 +8993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D618CA9B-8483-4F01-824C-AFC919087770}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7056,7 +10788,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7074,7 +10806,7 @@
         <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>193</v>
@@ -7158,7 +10890,7 @@
       <c r="H5" t="s">
         <v>196</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="13">
         <f ca="1">I4/B25</f>
         <v>0.83333333333333337</v>
       </c>
@@ -7597,12 +11329,674 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3921CD35-E3FB-4076-863C-CDE02BDE2C9B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="50.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3">
+        <f ca="1">_xlfn.CEILING.MATH(Model!B16/Model!B26)</f>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15">
+        <f ca="1">B32</f>
+        <v>-41000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4">
+        <f ca="1">B3*Model!B15</f>
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f ca="1">IF(F4=Model!$B$8,$B$34+$B$33,IF(F4&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>7386.3340000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" s="14">
+        <f ca="1">B4/Model!B25</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f ca="1">IF(F5=Model!$B$8,$B$34+$B$33,IF(F5&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>7386.3340000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="2">
+        <f ca="1">_xlfn.CEILING.MATH(B5/Model!B27)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f ca="1">IF(F6=Model!$B$8,$B$34+$B$33,IF(F6&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>7386.3340000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="15">
+        <f ca="1">Model!B20*Outputs!B6</f>
+        <v>74000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <f ca="1">IF(F7=Model!$B$8,$B$34+$B$33,IF(F7&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>7386.3340000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="15">
+        <f ca="1">Model!B21/100*Model!B5*Model!B17*Outputs!B4</f>
+        <v>246.66200000000003</v>
+      </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <f ca="1">IF(F8=Model!$B$8,$B$34+$B$33,IF(F8&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>7386.3340000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="15">
+        <f ca="1">B5*Model!B22*Model!B17</f>
+        <v>9010</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <f ca="1">IF(F9=Model!$B$8,$B$34+$B$33,IF(F9&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>7386.3340000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="15">
+        <f ca="1">(B9+B8)</f>
+        <v>9256.6620000000003</v>
+      </c>
+      <c r="C10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <f ca="1">IF(F10=Model!$B$8,$B$34+$B$33,IF(F10&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>5186.3340000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="15">
+        <f ca="1">12*Model!B23*B6</f>
+        <v>1440</v>
+      </c>
+      <c r="C11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <f ca="1">IF(F11=Model!$B$8,$B$34+$B$33,IF(F11&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="15">
+        <f ca="1">B11+B10</f>
+        <v>10696.662</v>
+      </c>
+      <c r="C12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <f ca="1">IF(F12=Model!$B$8,$B$34+$B$33,IF(F12&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" s="15">
+        <f ca="1">B12*Model!B8</f>
+        <v>74876.634000000005</v>
+      </c>
+      <c r="C13" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <f ca="1">IF(F13=Model!$B$8,$B$34+$B$33,IF(F13&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="15">
+        <f ca="1">B6*Model!B24</f>
+        <v>1800</v>
+      </c>
+      <c r="C14" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <f ca="1">IF(F14=Model!$B$8,$B$34+$B$33,IF(F14&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <f ca="1">IF(F15=Model!$B$8,$B$34+$B$33,IF(F15&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <f ca="1">IF(F16=Model!$B$8,$B$34+$B$33,IF(F16&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17">
+        <f ca="1">Model!B16/Model!B38</f>
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <f ca="1">IF(F17=Model!$B$8,$B$34+$B$33,IF(F17&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18">
+        <f ca="1">B17*Model!B15</f>
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <f ca="1">IF(F18=Model!$B$8,$B$34+$B$33,IF(F18&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" s="14">
+        <f ca="1">B18/Model!B34</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="C19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <f ca="1">IF(F19=Model!$B$8,$B$34+$B$33,IF(F19&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20">
+        <f ca="1">_xlfn.CEILING.MATH(B19/Model!B40)</f>
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20">
+        <f ca="1">IF(F20=Model!$B$8,$B$34+$B$33,IF(F20&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="15">
+        <f ca="1">B20*Model!B30</f>
+        <v>115000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21">
+        <f ca="1">IF(F21=Model!$B$8,$B$34+$B$33,IF(F21&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="15">
+        <f ca="1">Model!B4*Model!B39*Model!B17*Outputs!B18</f>
+        <v>136.52800000000002</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <f ca="1">IF(F22=Model!$B$8,$B$34+$B$33,IF(F22&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" s="15">
+        <f ca="1">Model!B41*Model!B7*Model!B17</f>
+        <v>593.59999999999991</v>
+      </c>
+      <c r="C23" t="s">
+        <v>217</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <f ca="1">IF(F23=Model!$B$8,$B$34+$B$33,IF(F23&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="15">
+        <f ca="1">Model!B37/60*Model!B22</f>
+        <v>4.25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>240</v>
+      </c>
+      <c r="F24">
+        <v>21</v>
+      </c>
+      <c r="G24">
+        <f ca="1">IF(F24=Model!$B$8,$B$34+$B$33,IF(F24&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" s="15">
+        <f ca="1">B24*Model!B36*Model!B17*Outputs!B18</f>
+        <v>180.2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25">
+        <v>22</v>
+      </c>
+      <c r="G25">
+        <f ca="1">IF(F25=Model!$B$8,$B$34+$B$33,IF(F25&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" s="15">
+        <f ca="1">B22+B23+B25</f>
+        <v>910.32799999999997</v>
+      </c>
+      <c r="C26" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <f ca="1">IF(F26=Model!$B$8,$B$34+$B$33,IF(F26&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>234</v>
+      </c>
+      <c r="B27" s="15">
+        <f ca="1">12*Model!B32</f>
+        <v>2400</v>
+      </c>
+      <c r="C27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F27">
+        <v>24</v>
+      </c>
+      <c r="G27">
+        <f ca="1">IF(F27=Model!$B$8,$B$34+$B$33,IF(F27&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" s="15">
+        <f ca="1">B20*(B27+B26)</f>
+        <v>3310.328</v>
+      </c>
+      <c r="C28" t="s">
+        <v>217</v>
+      </c>
+      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <f ca="1">IF(F28=Model!$B$8,$B$34+$B$33,IF(F28&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" s="15">
+        <f ca="1">B28*Model!B8</f>
+        <v>23172.295999999998</v>
+      </c>
+      <c r="C29" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <f ca="1">IF(F29=Model!$B$8,$B$34+$B$33,IF(F29&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>236</v>
+      </c>
+      <c r="B30" s="15">
+        <f ca="1">B20*Model!B33</f>
+        <v>4000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30">
+        <v>27</v>
+      </c>
+      <c r="G30">
+        <f ca="1">IF(F30=Model!$B$8,$B$34+$B$33,IF(F30&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>28</v>
+      </c>
+      <c r="G31">
+        <f ca="1">IF(F31=Model!$B$8,$B$34+$B$33,IF(F31&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B32" s="15">
+        <f ca="1">B7-B21</f>
+        <v>-41000</v>
+      </c>
+      <c r="F32">
+        <v>29</v>
+      </c>
+      <c r="G32">
+        <f ca="1">IF(F32=Model!$B$8,$B$34+$B$33,IF(F32&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>242</v>
+      </c>
+      <c r="B33" s="15">
+        <f ca="1">B12-B28</f>
+        <v>7386.3340000000007</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33">
+        <f ca="1">IF(F33=Model!$B$8,$B$34+$B$33,IF(F33&lt;=Model!$B$8-1,Outputs!$B$33,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B34" s="15">
+        <f ca="1">B14-B30</f>
+        <v>-2200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>244</v>
+      </c>
+      <c r="B37" s="15">
+        <f ca="1">B7+Model!B8*Outputs!B12+Outputs!B14</f>
+        <v>150676.63400000002</v>
+      </c>
+      <c r="C37" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B38" s="15">
+        <f ca="1">B21+Model!B8*Outputs!B28+Outputs!B30</f>
+        <v>142172.296</v>
+      </c>
+      <c r="C38" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" s="16">
+        <f ca="1">NPV(Model!B3,G3:G33)</f>
+        <v>168.1787005780028</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B44" s="17">
+        <f ca="1">NPER(Model!B3,Outputs!B33,Outputs!B32)</f>
+        <v>6.6630773081481927</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjusted sensitivity analysis to 1-9 TR level
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68311D03-52B2-4360-B61E-C07C55477BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43FCB03-590E-4742-89F1-949E546E4E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="9" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="264">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -849,6 +849,18 @@
   </si>
   <si>
     <t>Misson Determinism</t>
+  </si>
+  <si>
+    <t>Time Per Disengagement (min)</t>
+  </si>
+  <si>
+    <t>Average Speed (km/hr)</t>
+  </si>
+  <si>
+    <t>Disengagements Per Km (1/km)</t>
+  </si>
+  <si>
+    <t>Technology Level</t>
   </si>
 </sst>
 </file>
@@ -859,8 +871,8 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -963,9 +975,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -1742,6 +1754,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-754E-4126-A14A-C05D94A894FC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1757,6 +1774,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-754E-4126-A14A-C05D94A894FC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1772,6 +1794,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-754E-4126-A14A-C05D94A894FC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2218,6 +2245,766 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>InputSensitivity!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Technology readiness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.30362894361543336</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50918243748356329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85389341198670998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4319699686378955</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0271184552531007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.75343386787908</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.325435175198921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.992631662196889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBDB-4069-B525-DED8B3DE40F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>InputSensitivity!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Company Acceptance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$B$12:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$E$12:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FBDB-4069-B525-DED8B3DE40F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>InputSensitivity!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mission Similarity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$C$23:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$E$23:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.30017475868415672</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60034951736831343</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90052427605246999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2006990347366269</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5008737934207834</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.80104855210494</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1012233107890967</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7015728281574103</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0017475868415668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FBDB-4069-B525-DED8B3DE40F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>InputSensitivity!$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Misson Determinism</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$D$34:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>InputSensitivity!$E$34:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.40023301157887564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80046602315775128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2006990347366269</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6009320463155026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.001165057894378</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4013980694732537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.801631081052129</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2018640926310051</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6020971042098804</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0023301157887561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-FBDB-4069-B525-DED8B3DE40F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="844068000"/>
+        <c:axId val="844069080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="844068000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844069080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="844069080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844068000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2753,7 +3540,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -3310,7 +4097,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -4107,6 +4894,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6668,6 +7495,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7335,6 +8678,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EE7B598-38BF-C0F4-9B4E-283AE75D6B2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7907,10 +9291,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E08E8B2-3823-4F4D-943E-C68B1F535EDC}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7918,7 +9302,7 @@
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>258</v>
       </c>
@@ -7931,92 +9315,200 @@
       <c r="D1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0.7</v>
+      </c>
+      <c r="C2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>0.6</v>
+      </c>
+      <c r="E2">
+        <f>0.5*0.7544*EXP(0.517*A2)*C2*D2</f>
+        <v>0.30362894361543336</v>
+      </c>
+      <c r="F2">
+        <f>243.16 * EXP(-0.679*A2)</f>
+        <v>123.31223846651093</v>
+      </c>
+      <c r="G2">
+        <f>5.133*EXP(-1.083 *A2)/B2/D2</f>
+        <v>4.1379100903453514</v>
+      </c>
+      <c r="H2">
+        <f>A2/10</f>
         <v>0.1</v>
       </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-      <c r="D2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>0.7</v>
+      </c>
+      <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
+        <v>0.6</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="0">0.5*0.7544*EXP(0.517*A3)*C3*D3</f>
+        <v>0.50918243748356329</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="1">243.16 * EXP(-0.679*A3)</f>
+        <v>62.534578695598213</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="2">5.133*EXP(-1.083 *A3)/B3/D3</f>
+        <v>1.4010064220978744</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="3">A3/10</f>
         <v>0.2</v>
       </c>
-      <c r="C3">
-        <v>0.2</v>
-      </c>
-      <c r="D3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>0.7</v>
+      </c>
+      <c r="C4">
+        <v>0.8</v>
+      </c>
+      <c r="D4">
+        <v>0.6</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.85389341198670998</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>31.712777103612453</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.47435032465765103</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
-      <c r="C4">
-        <v>0.3</v>
-      </c>
-      <c r="D4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5">
+        <v>0.6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1.4319699686378955</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>16.082306023342515</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.16060471026670267</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="C5">
-        <v>0.4</v>
-      </c>
-      <c r="D5">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>0.7</v>
+      </c>
+      <c r="C6">
+        <v>0.8</v>
+      </c>
+      <c r="D6">
+        <v>0.6</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="C6">
-        <v>0.5</v>
-      </c>
-      <c r="D6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="C7">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.0271184552531007</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.135960814374922</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1.8410959830739128E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8024,53 +9516,940 @@
         <v>0.7</v>
       </c>
       <c r="C8">
+        <v>0.8</v>
+      </c>
+      <c r="D8">
+        <v>0.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>6.75343386787908</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2.0974444243722039</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>6.2335508497476152E-3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="D8">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="C9">
         <v>0.8</v>
       </c>
       <c r="D9">
+        <v>0.6</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>11.325435175198921</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.0636641183929878</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>2.1105448359901866E-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10">
+        <v>0.6</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>18.992631662196889</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.53940945638899163</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>7.1458461029562219E-4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="C10">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E11" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="C12">
+        <v>0.8</v>
+      </c>
+      <c r="D12">
+        <v>0.6</v>
+      </c>
+      <c r="E12">
+        <f>0.5*0.7544*EXP(0.517*A12)*C12*D12</f>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F12">
+        <f>243.16 * EXP(-0.679*A12)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G12">
+        <f>5.133*EXP(-1.083 *A12)/B12/D12</f>
+        <v>0.38064084988088182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>0.8</v>
+      </c>
+      <c r="D13">
+        <v>0.6</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E20" si="4">0.5*0.7544*EXP(0.517*A13)*C13*D13</f>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F20" si="5">243.16 * EXP(-0.679*A13)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G20" si="6">5.133*EXP(-1.083 *A13)/B13/D13</f>
+        <v>0.19032042494044091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14">
+        <v>0.6</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="6"/>
+        <v>0.12688028329362727</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>0.4</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>0.6</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="6"/>
+        <v>9.5160212470220454E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>0.8</v>
+      </c>
+      <c r="D16">
+        <v>0.6</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="6"/>
+        <v>7.6128169976176358E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0.6</v>
+      </c>
+      <c r="C17">
+        <v>0.8</v>
+      </c>
+      <c r="D17">
+        <v>0.6</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="6"/>
+        <v>6.3440141646813636E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>0.7</v>
+      </c>
+      <c r="C18">
+        <v>0.8</v>
+      </c>
+      <c r="D18">
+        <v>0.6</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="6"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>0.8</v>
+      </c>
+      <c r="C19">
+        <v>0.8</v>
+      </c>
+      <c r="D19">
+        <v>0.6</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>4.7580106235110227E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
         <v>0.9</v>
       </c>
-      <c r="D10">
+      <c r="C20">
+        <v>0.8</v>
+      </c>
+      <c r="D20">
+        <v>0.6</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="6"/>
+        <v>4.2293427764542417E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.8</v>
+      </c>
+      <c r="D21">
+        <v>0.6</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="7">0.5*0.7544*EXP(0.517*A21)*C21*D21</f>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21" si="8">243.16 * EXP(-0.679*A21)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21" si="9">5.133*EXP(-1.083 *A21)/B21/D21</f>
+        <v>3.8064084988088179E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22" t="s">
+        <v>261</v>
+      </c>
+      <c r="F22" t="s">
+        <v>260</v>
+      </c>
+      <c r="G22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>0.7</v>
+      </c>
+      <c r="C23">
+        <v>0.1</v>
+      </c>
+      <c r="D23">
+        <v>0.6</v>
+      </c>
+      <c r="E23">
+        <f>0.5*0.7544*EXP(0.517*A23)*C23*D23</f>
+        <v>0.30017475868415672</v>
+      </c>
+      <c r="F23">
+        <f>243.16 * EXP(-0.679*A23)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G23">
+        <f>5.133*EXP(-1.083 *A23)/B23/D23</f>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0.7</v>
+      </c>
+      <c r="C24">
+        <v>0.2</v>
+      </c>
+      <c r="D24">
+        <v>0.6</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E32" si="10">0.5*0.7544*EXP(0.517*A24)*C24*D24</f>
+        <v>0.60034951736831343</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ref="F24:F32" si="11">243.16 * EXP(-0.679*A24)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G32" si="12">5.133*EXP(-1.083 *A24)/B24/D24</f>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>0.7</v>
+      </c>
+      <c r="C25">
+        <v>0.3</v>
+      </c>
+      <c r="D25">
+        <v>0.6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="10"/>
+        <v>0.90052427605246999</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>0.7</v>
+      </c>
+      <c r="C26">
+        <v>0.4</v>
+      </c>
+      <c r="D26">
+        <v>0.6</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="10"/>
+        <v>1.2006990347366269</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>0.7</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>0.6</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="10"/>
+        <v>1.5008737934207834</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>0.7</v>
+      </c>
+      <c r="C28">
+        <v>0.6</v>
+      </c>
+      <c r="D28">
+        <v>0.6</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="10"/>
+        <v>1.80104855210494</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>0.7</v>
+      </c>
+      <c r="C29">
+        <v>0.7</v>
+      </c>
+      <c r="D29">
+        <v>0.6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="10"/>
+        <v>2.1012233107890967</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>0.7</v>
+      </c>
+      <c r="C30">
+        <v>0.8</v>
+      </c>
+      <c r="D30">
+        <v>0.6</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="10"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>0.7</v>
+      </c>
+      <c r="C31">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="D31">
+        <v>0.6</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="10"/>
+        <v>2.7015728281574103</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>0.7</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="D32">
+        <v>0.6</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="10"/>
+        <v>3.0017475868415668</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="11"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="12"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>258</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" t="s">
+        <v>259</v>
+      </c>
+      <c r="E33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F33" t="s">
+        <v>260</v>
+      </c>
+      <c r="G33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>0.7</v>
+      </c>
+      <c r="C34">
+        <v>0.8</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+      <c r="E34">
+        <f>0.5*0.7544*EXP(0.517*A34)*C34*D34</f>
+        <v>0.40023301157887564</v>
+      </c>
+      <c r="F34">
+        <f>243.16 * EXP(-0.679*A34)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G34">
+        <f>5.133*EXP(-1.083 *A34)/B34/D34</f>
+        <v>0.32626358561218438</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>0.7</v>
+      </c>
+      <c r="C35">
+        <v>0.8</v>
+      </c>
+      <c r="D35">
+        <v>0.2</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35:E43" si="13">0.5*0.7544*EXP(0.517*A35)*C35*D35</f>
+        <v>0.80046602315775128</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:F43" si="14">243.16 * EXP(-0.679*A35)</f>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35:G43" si="15">5.133*EXP(-1.083 *A35)/B35/D35</f>
+        <v>0.16313179280609219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>0.7</v>
+      </c>
+      <c r="C36">
+        <v>0.8</v>
+      </c>
+      <c r="D36">
+        <v>0.3</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="13"/>
+        <v>1.2006990347366269</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="15"/>
+        <v>0.10875452853739481</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>0.7</v>
+      </c>
+      <c r="C37">
+        <v>0.8</v>
+      </c>
+      <c r="D37">
+        <v>0.4</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="13"/>
+        <v>1.6009320463155026</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="15"/>
+        <v>8.1565896403046095E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>0.7</v>
+      </c>
+      <c r="C38">
+        <v>0.8</v>
+      </c>
+      <c r="D38">
+        <v>0.5</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="13"/>
+        <v>2.001165057894378</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="15"/>
+        <v>6.5252717122436882E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>0.7</v>
+      </c>
+      <c r="C39">
+        <v>0.8</v>
+      </c>
+      <c r="D39">
+        <v>0.6</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="13"/>
+        <v>2.4013980694732537</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="15"/>
+        <v>5.4377264268697406E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.7</v>
+      </c>
+      <c r="C40">
+        <v>0.8</v>
+      </c>
+      <c r="D40">
+        <v>0.7</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="13"/>
+        <v>2.801631081052129</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="15"/>
+        <v>4.6609083658883492E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>0.7</v>
+      </c>
+      <c r="C41">
+        <v>0.8</v>
+      </c>
+      <c r="D41">
+        <v>0.8</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="13"/>
+        <v>3.2018640926310051</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="15"/>
+        <v>4.0782948201523048E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>0.7</v>
+      </c>
+      <c r="C42">
+        <v>0.8</v>
+      </c>
+      <c r="D42">
+        <v>0.9</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="13"/>
+        <v>3.6020971042098804</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="15"/>
+        <v>3.6251509512464933E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>0.7</v>
+      </c>
+      <c r="C43">
+        <v>0.8</v>
+      </c>
+      <c r="D43">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>1</v>
+      <c r="E43">
+        <f t="shared" si="13"/>
+        <v>4.0023301157887561</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="14"/>
+        <v>8.1557211524996589</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="15"/>
+        <v>3.2626358561218441E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added the AGV use case model
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C793D27B-8534-4B2D-ACF3-2A7D50262A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F46EE0-C8E2-44AE-9FEF-07788212C0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="11" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
@@ -16222,8 +16222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8F2B30-5546-4786-948F-2BC73EA35898}">
   <dimension ref="A1:A74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added assumption sensitivity section
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F46EE0-C8E2-44AE-9FEF-07788212C0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2424137-8092-413C-855A-7395CB17280C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="11" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="283">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -912,6 +912,15 @@
   </si>
   <si>
     <t>AGV Cost</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Change from baseline</t>
+  </si>
+  <si>
+    <t>Baseline</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1179,7 @@
                   <c:v>150676.63400000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>142172.296</c:v>
+                  <c:v>142831.9327282928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1355,6 +1364,556 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Disengagement per km</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TechMaturity!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>disengagement per km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>3.3333333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>1.6666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>1.1111111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>8.3333333333333339E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TechMaturity!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>disengagement per km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.0253681195074532E-3"/>
+                  <c:y val="-0.19308852331403412"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>3.3333333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>1.6666666666666668E-3</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>1.1111111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>8.3333333333333339E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="844849416"/>
+        <c:axId val="844850496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="844849416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Technology</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Readiness Level</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844850496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="844850496"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Disengagements/km (LOG scale)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844849416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -1911,7 +2470,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -2611,25 +3170,25 @@
                   <c:v>-41000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>7292.1001816724565</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>7292.1001816724565</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>7292.1001816724565</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>7292.1001816724565</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>7292.1001816724565</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>7292.1001816724565</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5186.3340000000007</c:v>
+                  <c:v>5092.1001816724565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3279,7 +3838,7 @@
                   <c:v>115000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23172.295999999998</c:v>
+                  <c:v>23831.932728292806</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
@@ -7427,9 +7986,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-CA"/>
-              <a:t>Disengagement per km</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>The impact of AGV</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Cost on Net Present Value</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -7441,6 +8005,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -7449,108 +8033,15 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TechMaturity!$I$1</c:f>
+              <c:f>AssumptionSensitivity!$C$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>disengagement per km</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>TechMaturity!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>TechMaturity!$I$2:$I$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0000">
-                  <c:v>6.6666666666666671E-3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.0000">
-                  <c:v>3.3333333333333335E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.0000">
-                  <c:v>1.6666666666666668E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.0000">
-                  <c:v>1.1111111111111111E-3</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.0000">
-                  <c:v>8.3333333333333339E-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-C3AC-4F06-A5B4-ADD91AD596D7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>TechMaturity!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>disengagement per km</c:v>
+                  <c:v>NPV</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7579,124 +8070,62 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="9.0253681195074532E-3"/>
-                  <c:y val="-0.19308852331403412"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>TechMaturity!$A$2:$A$10</c:f>
+              <c:f>AssumptionSensitivity!$B$58:$B$64</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>-0.32608695652173914</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>-0.15217391304347827</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>2.1739130434782608E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0.19565217391304349</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>0.36956521739130432</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>0.54347826086956519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TechMaturity!$I$2:$I$10</c:f>
+              <c:f>AssumptionSensitivity!$C$58:$C$64</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* "-"??\ [$CHF-100C]_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>54410.776739144007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>35363.157691524953</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>16315.538643905906</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0000">
-                  <c:v>6.6666666666666671E-3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.0000">
-                  <c:v>3.3333333333333335E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.0000">
-                  <c:v>1.6666666666666668E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.0000">
-                  <c:v>1.1111111111111111E-3</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.0000">
-                  <c:v>8.3333333333333339E-4</c:v>
+                  <c:v>-2732.0804037131415</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-21779.699451332181</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-40827.318498951237</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-59874.937546570283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7704,7 +8133,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-C3AC-4F06-A5B4-ADD91AD596D7}"/>
+              <c16:uniqueId val="{00000000-AE9E-43FF-8360-ED5296A2E262}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7716,11 +8145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="844849416"/>
-        <c:axId val="844850496"/>
+        <c:axId val="915969712"/>
+        <c:axId val="911674992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="844849416"/>
+        <c:axId val="915969712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7761,11 +8190,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Technology</a:t>
+                  <a:t>%</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-CA" baseline="0"/>
-                  <a:t> Readiness Level</a:t>
+                  <a:t> Change from Baseline</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-CA"/>
               </a:p>
@@ -7779,8 +8208,28 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7817,14 +8266,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="844850496"/>
+        <c:crossAx val="911674992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="844850496"/>
+        <c:axId val="911674992"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -7864,8 +8312,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Disengagements/km (LOG scale)</a:t>
+                  <a:t>Net</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Present Value (CHF)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -7877,10 +8330,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -7915,16 +8388,44 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="844849416"/>
+        <c:crossAx val="915969712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -7984,6 +8485,46 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9362,6 +9903,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -13802,8 +14859,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>278731</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>193006</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>96593</xdr:rowOff>
     </xdr:to>
@@ -13880,6 +14937,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9634AED-482C-B55C-1707-69E14F9C7700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -16220,13 +17313,18 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8F2B30-5546-4786-948F-2BC73EA35898}">
-  <dimension ref="A1:A74"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -16243,116 +17341,113 @@
         <v>278</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>282</v>
+      </c>
+      <c r="C56">
+        <v>115000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="B57" t="s">
+        <v>281</v>
+      </c>
+      <c r="C57" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
         <v>57500</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f>A57+100000</f>
+      <c r="B58" s="8">
+        <f>(A58-$C$56)/$C$56</f>
+        <v>-0.5</v>
+      </c>
+      <c r="C58" s="18">
+        <v>54410.776739144007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="18">
+        <f>A58+20000</f>
+        <v>77500</v>
+      </c>
+      <c r="B59" s="8">
+        <f t="shared" ref="B59:B64" si="0">(A59-$C$56)/$C$56</f>
+        <v>-0.32608695652173914</v>
+      </c>
+      <c r="C59" s="18">
+        <v>35363.157691524953</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="18">
+        <f t="shared" ref="A60:A64" si="1">A59+20000</f>
+        <v>97500</v>
+      </c>
+      <c r="B60" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.15217391304347827</v>
+      </c>
+      <c r="C60" s="18">
+        <v>16315.538643905906</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="18">
+        <f t="shared" si="1"/>
+        <v>117500</v>
+      </c>
+      <c r="B61" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1739130434782608E-2</v>
+      </c>
+      <c r="C61" s="18">
+        <v>-2732.0804037131415</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="18">
+        <f t="shared" si="1"/>
+        <v>137500</v>
+      </c>
+      <c r="B62" s="8">
+        <f t="shared" si="0"/>
+        <v>0.19565217391304349</v>
+      </c>
+      <c r="C62" s="18">
+        <v>-21779.699451332181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="18">
+        <f t="shared" si="1"/>
         <v>157500</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <f t="shared" ref="A59:A74" si="0">A58+100000</f>
-        <v>257500</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="B63" s="8">
         <f t="shared" si="0"/>
-        <v>357500</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
+        <v>0.36956521739130432</v>
+      </c>
+      <c r="C63" s="18">
+        <v>-40827.318498951237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="18">
+        <f t="shared" si="1"/>
+        <v>177500</v>
+      </c>
+      <c r="B64" s="8">
         <f t="shared" si="0"/>
-        <v>457500</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>557500</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>657500</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>757500</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>857500</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>957500</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <f t="shared" si="0"/>
-        <v>1057500</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <f t="shared" si="0"/>
-        <v>1157500</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <f t="shared" si="0"/>
-        <v>1257500</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <f t="shared" si="0"/>
-        <v>1357500</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <f>A70+100000</f>
-        <v>1457500</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <f t="shared" si="0"/>
-        <v>1557500</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <f t="shared" si="0"/>
-        <v>1657500</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <f t="shared" si="0"/>
-        <v>1757500</v>
+        <v>0.54347826086956519</v>
+      </c>
+      <c r="C64" s="18">
+        <v>-59874.937546570283</v>
       </c>
     </row>
   </sheetData>
@@ -18791,7 +19886,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19259,7 +20354,7 @@
         <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>193</v>
@@ -19673,7 +20768,7 @@
       </c>
       <c r="B34" s="10" cm="1">
         <f t="array" aca="1" ref="B34" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B34")</f>
-        <v>4</v>
+        <v>4.0271184552531007</v>
       </c>
       <c r="C34" t="s">
         <v>167</v>
@@ -19697,7 +20792,7 @@
       </c>
       <c r="B36" s="10" cm="1">
         <f t="array" aca="1" ref="B36" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B36")</f>
-        <v>0.01</v>
+        <v>1.8410959830739128E-2</v>
       </c>
       <c r="C36" t="s">
         <v>184</v>
@@ -19709,7 +20804,7 @@
       </c>
       <c r="B37" s="10" cm="1">
         <f t="array" aca="1" ref="B37" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B37")</f>
-        <v>5</v>
+        <v>4.135960814374922</v>
       </c>
       <c r="C37" t="s">
         <v>185</v>
@@ -19849,7 +20944,7 @@
       </c>
       <c r="G4">
         <f ca="1">IF(F4=ModelInput!$B$8,$B$34+$B$33,IF(F4&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -19868,7 +20963,7 @@
       </c>
       <c r="G5">
         <f ca="1">IF(F5=ModelInput!$B$8,$B$34+$B$33,IF(F5&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -19887,7 +20982,7 @@
       </c>
       <c r="G6">
         <f ca="1">IF(F6=ModelInput!$B$8,$B$34+$B$33,IF(F6&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -19906,7 +21001,7 @@
       </c>
       <c r="G7">
         <f ca="1">IF(F7=ModelInput!$B$8,$B$34+$B$33,IF(F7&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -19925,7 +21020,7 @@
       </c>
       <c r="G8">
         <f ca="1">IF(F8=ModelInput!$B$8,$B$34+$B$33,IF(F8&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -19944,7 +21039,7 @@
       </c>
       <c r="G9">
         <f ca="1">IF(F9=ModelInput!$B$8,$B$34+$B$33,IF(F9&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -19963,7 +21058,7 @@
       </c>
       <c r="G10">
         <f ca="1">IF(F10=ModelInput!$B$8,$B$34+$B$33,IF(F10&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>5186.3340000000007</v>
+        <v>5092.1001816724565</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -20107,7 +21202,7 @@
       </c>
       <c r="B19" s="14">
         <f ca="1">B18/ModelInput!B34</f>
-        <v>5</v>
+        <v>4.9663301991803515</v>
       </c>
       <c r="C19" t="s">
         <v>199</v>
@@ -20202,7 +21297,7 @@
       </c>
       <c r="B24" s="15">
         <f ca="1">ModelInput!B37/60*ModelInput!B22</f>
-        <v>4.25</v>
+        <v>3.5155666922186835</v>
       </c>
       <c r="C24" t="s">
         <v>240</v>
@@ -20221,7 +21316,7 @@
       </c>
       <c r="B25" s="15">
         <f ca="1">B24*ModelInput!B36*ModelInput!B17*ModelOutput!B18</f>
-        <v>180.2</v>
+        <v>274.43381832754386</v>
       </c>
       <c r="C25" t="s">
         <v>217</v>
@@ -20240,7 +21335,7 @@
       </c>
       <c r="B26" s="15">
         <f ca="1">B22+B23+B25</f>
-        <v>910.32799999999997</v>
+        <v>1004.5618183275437</v>
       </c>
       <c r="C26" t="s">
         <v>217</v>
@@ -20278,7 +21373,7 @@
       </c>
       <c r="B28" s="15">
         <f ca="1">B20*(B27+B26)</f>
-        <v>3310.328</v>
+        <v>3404.5618183275437</v>
       </c>
       <c r="C28" t="s">
         <v>217</v>
@@ -20297,7 +21392,7 @@
       </c>
       <c r="B29" s="15">
         <f ca="1">B28*ModelInput!B8</f>
-        <v>23172.295999999998</v>
+        <v>23831.932728292806</v>
       </c>
       <c r="C29" t="s">
         <v>164</v>
@@ -20360,7 +21455,7 @@
       </c>
       <c r="B33" s="15">
         <f ca="1">B12-B28</f>
-        <v>7386.3340000000007</v>
+        <v>7292.1001816724565</v>
       </c>
       <c r="F33">
         <v>30</v>
@@ -20405,7 +21500,7 @@
       </c>
       <c r="B38" s="15">
         <f ca="1">B21+ModelInput!B8*ModelOutput!B28+ModelOutput!B30</f>
-        <v>142172.296</v>
+        <v>142831.9327282928</v>
       </c>
       <c r="C38" t="s">
         <v>164</v>
@@ -20425,7 +21520,7 @@
       </c>
       <c r="B41" s="16">
         <f ca="1">NPV(ModelInput!B3,G3:G33)</f>
-        <v>168.1787005780028</v>
+        <v>-351.1280227607607</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>164</v>
@@ -20442,7 +21537,7 @@
       </c>
       <c r="B44" s="17">
         <f ca="1">NPER(ModelInput!B3,ModelOutput!B33,ModelOutput!B32)</f>
-        <v>6.6630773081481927</v>
+        <v>6.7650803158726109</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
basic AGV use case model
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2424137-8092-413C-855A-7395CB17280C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9308E65-8788-4CF8-8464-0AC4FA758138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="11" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="283">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -927,8 +927,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -1018,7 +1017,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1039,9 +1038,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1179,7 +1179,7 @@
                   <c:v>150676.63400000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>142831.9327282928</c:v>
+                  <c:v>142172.296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3170,25 +3170,25 @@
                   <c:v>-41000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7292.1001816724565</c:v>
+                  <c:v>7386.3340000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7292.1001816724565</c:v>
+                  <c:v>7386.3340000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7292.1001816724565</c:v>
+                  <c:v>7386.3340000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7292.1001816724565</c:v>
+                  <c:v>7386.3340000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7292.1001816724565</c:v>
+                  <c:v>7386.3340000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7292.1001816724565</c:v>
+                  <c:v>7386.3340000000007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5092.1001816724565</c:v>
+                  <c:v>5186.3340000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3838,7 +3838,7 @@
                   <c:v>115000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23831.932728292806</c:v>
+                  <c:v>23172.295999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
@@ -16940,7 +16940,7 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>-30660379.26628283</v>
       </c>
       <c r="C9">
@@ -16952,7 +16952,7 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>-3608424.0743925855</v>
       </c>
       <c r="C10">
@@ -16964,7 +16964,7 @@
       <c r="A11">
         <v>3</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>-297607.68853009638</v>
       </c>
       <c r="C11">
@@ -16976,7 +16976,7 @@
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>-50137.726831554013</v>
       </c>
       <c r="C12">
@@ -16988,7 +16988,7 @@
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>-7646.8577474220256</v>
       </c>
       <c r="C13">
@@ -17000,7 +17000,7 @@
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>-351.1280227607607</v>
       </c>
       <c r="C14">
@@ -17012,7 +17012,7 @@
       <c r="A15">
         <v>7</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <v>901.55692726733912</v>
       </c>
       <c r="C15">
@@ -17024,7 +17024,7 @@
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="17">
         <v>1116.6443336336306</v>
       </c>
       <c r="C16">
@@ -17036,7 +17036,7 @@
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <v>1153.5750817649459</v>
       </c>
       <c r="C17">
@@ -17053,7 +17053,7 @@
       <c r="A20">
         <v>0.1</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="17">
         <v>849.1267821900467</v>
       </c>
     </row>
@@ -17061,7 +17061,7 @@
       <c r="A21">
         <v>0.2</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>1005.1786871988046</v>
       </c>
     </row>
@@ -17069,7 +17069,7 @@
       <c r="A22">
         <v>0.3</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>1057.1959888683969</v>
       </c>
     </row>
@@ -17077,7 +17077,7 @@
       <c r="A23">
         <v>0.4</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <v>1083.2046397031861</v>
       </c>
     </row>
@@ -17085,7 +17085,7 @@
       <c r="A24">
         <v>0.5</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <v>1098.8098302040587</v>
       </c>
     </row>
@@ -17093,7 +17093,7 @@
       <c r="A25">
         <v>0.6</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="17">
         <v>1109.2132905379747</v>
       </c>
     </row>
@@ -17101,7 +17101,7 @@
       <c r="A26">
         <v>0.7</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="17">
         <v>1116.6443336336306</v>
       </c>
     </row>
@@ -17109,7 +17109,7 @@
       <c r="A27">
         <v>0.8</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="17">
         <v>1122.2176159553687</v>
       </c>
     </row>
@@ -17117,7 +17117,7 @@
       <c r="A28">
         <v>0.9</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <v>1126.5523910945069</v>
       </c>
     </row>
@@ -17125,7 +17125,7 @@
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <v>1130.0202112058078</v>
       </c>
     </row>
@@ -17141,7 +17141,7 @@
       <c r="A32">
         <v>0.1</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="17">
         <v>-130002.65604644013</v>
       </c>
       <c r="C32" t="s">
@@ -17152,7 +17152,7 @@
       <c r="A33">
         <v>0.2</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17160,7 +17160,7 @@
       <c r="A34">
         <v>0.3</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17168,7 +17168,7 @@
       <c r="A35">
         <v>0.4</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17176,7 +17176,7 @@
       <c r="A36">
         <v>0.5</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17184,7 +17184,7 @@
       <c r="A37">
         <v>0.6</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17192,7 +17192,7 @@
       <c r="A38">
         <v>0.7</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17200,7 +17200,7 @@
       <c r="A39">
         <v>0.8</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17208,7 +17208,7 @@
       <c r="A40">
         <v>0.9</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17216,7 +17216,7 @@
       <c r="A41">
         <v>1</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="17">
         <v>319.67523010741735</v>
       </c>
     </row>
@@ -17229,7 +17229,7 @@
       <c r="A44">
         <v>0.1</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="17">
         <v>893.71304076397655</v>
       </c>
     </row>
@@ -17237,7 +17237,7 @@
       <c r="A45">
         <v>0.2</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="17">
         <v>1027.471816485772</v>
       </c>
     </row>
@@ -17245,7 +17245,7 @@
       <c r="A46">
         <v>0.3</v>
       </c>
-      <c r="B46" s="18">
+      <c r="B46" s="17">
         <v>1072.0580750597019</v>
       </c>
     </row>
@@ -17253,7 +17253,7 @@
       <c r="A47">
         <v>0.4</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B47" s="17">
         <v>1094.351204346664</v>
       </c>
     </row>
@@ -17261,7 +17261,7 @@
       <c r="A48">
         <v>0.5</v>
       </c>
-      <c r="B48" s="18">
+      <c r="B48" s="17">
         <v>1107.7270819188439</v>
       </c>
     </row>
@@ -17269,7 +17269,7 @@
       <c r="A49">
         <v>0.6</v>
       </c>
-      <c r="B49" s="18">
+      <c r="B49" s="17">
         <v>1116.6443336336306</v>
       </c>
     </row>
@@ -17277,7 +17277,7 @@
       <c r="A50">
         <v>0.7</v>
       </c>
-      <c r="B50" s="18">
+      <c r="B50" s="17">
         <v>1123.0137991441984</v>
       </c>
     </row>
@@ -17285,7 +17285,7 @@
       <c r="A51">
         <v>0.8</v>
       </c>
-      <c r="B51" s="18">
+      <c r="B51" s="17">
         <v>1127.7908982771135</v>
       </c>
     </row>
@@ -17293,7 +17293,7 @@
       <c r="A52">
         <v>0.9</v>
       </c>
-      <c r="B52" s="18">
+      <c r="B52" s="17">
         <v>1131.5064198249374</v>
       </c>
     </row>
@@ -17301,7 +17301,7 @@
       <c r="A53">
         <v>1</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B53" s="17">
         <v>1134.4788370632041</v>
       </c>
     </row>
@@ -17315,7 +17315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8F2B30-5546-4786-948F-2BC73EA35898}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
@@ -17361,19 +17361,19 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="18">
+      <c r="A58" s="17">
         <v>57500</v>
       </c>
       <c r="B58" s="8">
         <f>(A58-$C$56)/$C$56</f>
         <v>-0.5</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="17">
         <v>54410.776739144007</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="18">
+      <c r="A59" s="17">
         <f>A58+20000</f>
         <v>77500</v>
       </c>
@@ -17381,12 +17381,12 @@
         <f t="shared" ref="B59:B64" si="0">(A59-$C$56)/$C$56</f>
         <v>-0.32608695652173914</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C59" s="17">
         <v>35363.157691524953</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="18">
+      <c r="A60" s="17">
         <f t="shared" ref="A60:A64" si="1">A59+20000</f>
         <v>97500</v>
       </c>
@@ -17394,12 +17394,12 @@
         <f t="shared" si="0"/>
         <v>-0.15217391304347827</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C60" s="17">
         <v>16315.538643905906</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="18">
+      <c r="A61" s="17">
         <f t="shared" si="1"/>
         <v>117500</v>
       </c>
@@ -17407,12 +17407,12 @@
         <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C61" s="17">
         <v>-2732.0804037131415</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="18">
+      <c r="A62" s="17">
         <f t="shared" si="1"/>
         <v>137500</v>
       </c>
@@ -17420,12 +17420,12 @@
         <f t="shared" si="0"/>
         <v>0.19565217391304349</v>
       </c>
-      <c r="C62" s="18">
+      <c r="C62" s="17">
         <v>-21779.699451332181</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="18">
+      <c r="A63" s="17">
         <f t="shared" si="1"/>
         <v>157500</v>
       </c>
@@ -17433,12 +17433,12 @@
         <f t="shared" si="0"/>
         <v>0.36956521739130432</v>
       </c>
-      <c r="C63" s="18">
+      <c r="C63" s="17">
         <v>-40827.318498951237</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="18">
+      <c r="A64" s="17">
         <f t="shared" si="1"/>
         <v>177500</v>
       </c>
@@ -17446,7 +17446,7 @@
         <f t="shared" si="0"/>
         <v>0.54347826086956519</v>
       </c>
-      <c r="C64" s="18">
+      <c r="C64" s="17">
         <v>-59874.937546570283</v>
       </c>
     </row>
@@ -18248,10 +18248,13 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="140" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -18259,27 +18262,39 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -19886,13 +19901,13 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20354,7 +20369,7 @@
         <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>193</v>
@@ -20505,7 +20520,7 @@
       <c r="A10" t="s">
         <v>143</v>
       </c>
-      <c r="B10" s="10" cm="1">
+      <c r="B10" s="8" cm="1">
         <f t="array" aca="1" ref="B10" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B10")</f>
         <v>0.7</v>
       </c>
@@ -20517,7 +20532,7 @@
       <c r="A11" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="10" cm="1">
+      <c r="B11" s="8" cm="1">
         <f t="array" aca="1" ref="B11" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B11")</f>
         <v>0.8</v>
       </c>
@@ -20529,7 +20544,7 @@
       <c r="A12" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="10" cm="1">
+      <c r="B12" s="8" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B12")</f>
         <v>0.6</v>
       </c>
@@ -20547,7 +20562,9 @@
       <c r="A14" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="10"/>
+      <c r="B14" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>125</v>
       </c>
@@ -20598,7 +20615,9 @@
       <c r="A19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>125</v>
       </c>
@@ -20709,7 +20728,9 @@
       <c r="A29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C29" s="2" t="s">
         <v>125</v>
       </c>
@@ -20768,7 +20789,7 @@
       </c>
       <c r="B34" s="10" cm="1">
         <f t="array" aca="1" ref="B34" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B34")</f>
-        <v>4.0271184552531007</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>167</v>
@@ -20792,7 +20813,7 @@
       </c>
       <c r="B36" s="10" cm="1">
         <f t="array" aca="1" ref="B36" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B36")</f>
-        <v>1.8410959830739128E-2</v>
+        <v>0.01</v>
       </c>
       <c r="C36" t="s">
         <v>184</v>
@@ -20804,7 +20825,7 @@
       </c>
       <c r="B37" s="10" cm="1">
         <f t="array" aca="1" ref="B37" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B37")</f>
-        <v>4.135960814374922</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
         <v>185</v>
@@ -20879,8 +20900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3921CD35-E3FB-4076-863C-CDE02BDE2C9B}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20944,7 +20965,7 @@
       </c>
       <c r="G4">
         <f ca="1">IF(F4=ModelInput!$B$8,$B$34+$B$33,IF(F4&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -20963,7 +20984,7 @@
       </c>
       <c r="G5">
         <f ca="1">IF(F5=ModelInput!$B$8,$B$34+$B$33,IF(F5&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -20982,7 +21003,7 @@
       </c>
       <c r="G6">
         <f ca="1">IF(F6=ModelInput!$B$8,$B$34+$B$33,IF(F6&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -21001,7 +21022,7 @@
       </c>
       <c r="G7">
         <f ca="1">IF(F7=ModelInput!$B$8,$B$34+$B$33,IF(F7&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -21020,7 +21041,7 @@
       </c>
       <c r="G8">
         <f ca="1">IF(F8=ModelInput!$B$8,$B$34+$B$33,IF(F8&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -21039,7 +21060,7 @@
       </c>
       <c r="G9">
         <f ca="1">IF(F9=ModelInput!$B$8,$B$34+$B$33,IF(F9&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -21058,7 +21079,7 @@
       </c>
       <c r="G10">
         <f ca="1">IF(F10=ModelInput!$B$8,$B$34+$B$33,IF(F10&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>5092.1001816724565</v>
+        <v>5186.3340000000007</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -21202,7 +21223,7 @@
       </c>
       <c r="B19" s="14">
         <f ca="1">B18/ModelInput!B34</f>
-        <v>4.9663301991803515</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
         <v>199</v>
@@ -21297,7 +21318,7 @@
       </c>
       <c r="B24" s="15">
         <f ca="1">ModelInput!B37/60*ModelInput!B22</f>
-        <v>3.5155666922186835</v>
+        <v>4.25</v>
       </c>
       <c r="C24" t="s">
         <v>240</v>
@@ -21316,7 +21337,7 @@
       </c>
       <c r="B25" s="15">
         <f ca="1">B24*ModelInput!B36*ModelInput!B17*ModelOutput!B18</f>
-        <v>274.43381832754386</v>
+        <v>180.2</v>
       </c>
       <c r="C25" t="s">
         <v>217</v>
@@ -21335,7 +21356,7 @@
       </c>
       <c r="B26" s="15">
         <f ca="1">B22+B23+B25</f>
-        <v>1004.5618183275437</v>
+        <v>910.32799999999997</v>
       </c>
       <c r="C26" t="s">
         <v>217</v>
@@ -21373,7 +21394,7 @@
       </c>
       <c r="B28" s="15">
         <f ca="1">B20*(B27+B26)</f>
-        <v>3404.5618183275437</v>
+        <v>3310.328</v>
       </c>
       <c r="C28" t="s">
         <v>217</v>
@@ -21392,7 +21413,7 @@
       </c>
       <c r="B29" s="15">
         <f ca="1">B28*ModelInput!B8</f>
-        <v>23831.932728292806</v>
+        <v>23172.295999999998</v>
       </c>
       <c r="C29" t="s">
         <v>164</v>
@@ -21455,7 +21476,7 @@
       </c>
       <c r="B33" s="15">
         <f ca="1">B12-B28</f>
-        <v>7292.1001816724565</v>
+        <v>7386.3340000000007</v>
       </c>
       <c r="F33">
         <v>30</v>
@@ -21500,7 +21521,7 @@
       </c>
       <c r="B38" s="15">
         <f ca="1">B21+ModelInput!B8*ModelOutput!B28+ModelOutput!B30</f>
-        <v>142831.9327282928</v>
+        <v>142172.296</v>
       </c>
       <c r="C38" t="s">
         <v>164</v>
@@ -21518,11 +21539,11 @@
       <c r="A41" t="s">
         <v>247</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="19">
         <f ca="1">NPV(ModelInput!B3,G3:G33)</f>
-        <v>-351.1280227607607</v>
-      </c>
-      <c r="C41" s="2" t="s">
+        <v>168.1787005780028</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>164</v>
       </c>
     </row>
@@ -21535,9 +21556,9 @@
       <c r="A44" t="s">
         <v>252</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="16">
         <f ca="1">NPER(ModelInput!B3,ModelOutput!B33,ModelOutput!B32)</f>
-        <v>6.7650803158726109</v>
+        <v>6.6630773081481927</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
started filling in the kemaro case numbers, need to add ROI diagram
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9308E65-8788-4CF8-8464-0AC4FA758138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E57D3C8-BB62-481D-9CC9-5D0706FE5187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
@@ -1176,10 +1176,10 @@
                 <c:formatCode>_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>150676.63400000002</c:v>
+                  <c:v>34393.324000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>142172.296</c:v>
+                  <c:v>29821.923636655087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3167,28 +3167,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-">
-                  <c:v>-41000</c:v>
+                  <c:v>-13000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>8785.7001816724569</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>8785.7001816724569</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7386.3340000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5186.3340000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3550,13 +3550,13 @@
                 <c:formatCode>_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>74000</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74876.634000000005</c:v>
+                  <c:v>21393.324000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1800</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3835,13 +3835,13 @@
                 <c:formatCode>_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>115000</c:v>
+                  <c:v>26000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23172.295999999998</c:v>
+                  <c:v>3821.9236366550876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19900,8 +19900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1938A5B1-C94B-40F6-B37D-6D55F3EDC6C6}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19987,7 +19987,7 @@
         <v>139</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>140</v>
@@ -20107,7 +20107,7 @@
         <v>163</v>
       </c>
       <c r="B20">
-        <v>74000</v>
+        <v>13000</v>
       </c>
       <c r="C20" t="s">
         <v>164</v>
@@ -20151,7 +20151,7 @@
         <v>158</v>
       </c>
       <c r="B24">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>164</v>
@@ -20211,7 +20211,7 @@
         <v>162</v>
       </c>
       <c r="B30">
-        <v>115000</v>
+        <v>26000</v>
       </c>
       <c r="C30" t="s">
         <v>164</v>
@@ -20233,7 +20233,8 @@
         <v>170</v>
       </c>
       <c r="B32">
-        <v>200</v>
+        <f>1500/12</f>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
         <v>182</v>
@@ -20244,7 +20245,7 @@
         <v>171</v>
       </c>
       <c r="B33">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>164</v>
@@ -20335,7 +20336,7 @@
         <v>179</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
         <v>187</v>
@@ -20369,7 +20370,7 @@
         <v>128</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>193</v>
@@ -20498,7 +20499,7 @@
       </c>
       <c r="B8" s="10" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B8")</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>140</v>
@@ -20628,7 +20629,7 @@
       </c>
       <c r="B20" s="10" cm="1">
         <f t="array" aca="1" ref="B20" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B20")</f>
-        <v>74000</v>
+        <v>13000</v>
       </c>
       <c r="C20" t="s">
         <v>164</v>
@@ -20676,7 +20677,7 @@
       </c>
       <c r="B24" s="10" cm="1">
         <f t="array" aca="1" ref="B24" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B24")</f>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>164</v>
@@ -20741,7 +20742,7 @@
       </c>
       <c r="B30" s="10" cm="1">
         <f t="array" aca="1" ref="B30" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B30")</f>
-        <v>115000</v>
+        <v>26000</v>
       </c>
       <c r="C30" t="s">
         <v>164</v>
@@ -20765,7 +20766,7 @@
       </c>
       <c r="B32" s="10" cm="1">
         <f t="array" aca="1" ref="B32" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B32")</f>
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
         <v>182</v>
@@ -20777,7 +20778,7 @@
       </c>
       <c r="B33" s="10" cm="1">
         <f t="array" aca="1" ref="B33" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B33")</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
         <v>164</v>
@@ -20789,7 +20790,7 @@
       </c>
       <c r="B34" s="10" cm="1">
         <f t="array" aca="1" ref="B34" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B34")</f>
-        <v>4</v>
+        <v>4.0271184552531007</v>
       </c>
       <c r="C34" t="s">
         <v>167</v>
@@ -20813,7 +20814,7 @@
       </c>
       <c r="B36" s="10" cm="1">
         <f t="array" aca="1" ref="B36" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B36")</f>
-        <v>0.01</v>
+        <v>1.8410959830739128E-2</v>
       </c>
       <c r="C36" t="s">
         <v>184</v>
@@ -20825,7 +20826,7 @@
       </c>
       <c r="B37" s="10" cm="1">
         <f t="array" aca="1" ref="B37" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B37")</f>
-        <v>5</v>
+        <v>4.135960814374922</v>
       </c>
       <c r="C37" t="s">
         <v>185</v>
@@ -20873,7 +20874,7 @@
       </c>
       <c r="B41" s="10" cm="1">
         <f t="array" aca="1" ref="B41" ca="1">INDIRECT("'"&amp;$F$1&amp;"'!B41")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
         <v>187</v>
@@ -20901,7 +20902,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20946,7 +20947,7 @@
       </c>
       <c r="G3" s="15">
         <f ca="1">B32</f>
-        <v>-41000</v>
+        <v>-13000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -20965,7 +20966,7 @@
       </c>
       <c r="G4">
         <f ca="1">IF(F4=ModelInput!$B$8,$B$34+$B$33,IF(F4&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>8785.7001816724569</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -20984,7 +20985,7 @@
       </c>
       <c r="G5">
         <f ca="1">IF(F5=ModelInput!$B$8,$B$34+$B$33,IF(F5&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>8785.7001816724569</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -21003,7 +21004,7 @@
       </c>
       <c r="G6">
         <f ca="1">IF(F6=ModelInput!$B$8,$B$34+$B$33,IF(F6&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -21012,7 +21013,7 @@
       </c>
       <c r="B7" s="15">
         <f ca="1">ModelInput!B20*ModelOutput!B6</f>
-        <v>74000</v>
+        <v>13000</v>
       </c>
       <c r="C7" t="s">
         <v>223</v>
@@ -21022,7 +21023,7 @@
       </c>
       <c r="G7">
         <f ca="1">IF(F7=ModelInput!$B$8,$B$34+$B$33,IF(F7&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -21041,7 +21042,7 @@
       </c>
       <c r="G8">
         <f ca="1">IF(F8=ModelInput!$B$8,$B$34+$B$33,IF(F8&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -21060,7 +21061,7 @@
       </c>
       <c r="G9">
         <f ca="1">IF(F9=ModelInput!$B$8,$B$34+$B$33,IF(F9&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>7386.3340000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -21079,7 +21080,7 @@
       </c>
       <c r="G10">
         <f ca="1">IF(F10=ModelInput!$B$8,$B$34+$B$33,IF(F10&lt;=ModelInput!$B$8-1,ModelOutput!$B$33,0))</f>
-        <v>5186.3340000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -21126,7 +21127,7 @@
       </c>
       <c r="B13" s="15">
         <f ca="1">B12*ModelInput!B8</f>
-        <v>74876.634000000005</v>
+        <v>21393.324000000001</v>
       </c>
       <c r="C13" t="s">
         <v>164</v>
@@ -21145,7 +21146,7 @@
       </c>
       <c r="B14" s="15">
         <f ca="1">B6*ModelInput!B24</f>
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>164</v>
@@ -21223,7 +21224,7 @@
       </c>
       <c r="B19" s="14">
         <f ca="1">B18/ModelInput!B34</f>
-        <v>5</v>
+        <v>4.9663301991803515</v>
       </c>
       <c r="C19" t="s">
         <v>199</v>
@@ -21261,7 +21262,7 @@
       </c>
       <c r="B21" s="15">
         <f ca="1">B20*ModelInput!B30</f>
-        <v>115000</v>
+        <v>26000</v>
       </c>
       <c r="C21" t="s">
         <v>223</v>
@@ -21299,7 +21300,7 @@
       </c>
       <c r="B23" s="15">
         <f ca="1">ModelInput!B41*ModelInput!B7*ModelInput!B17</f>
-        <v>593.59999999999991</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
         <v>217</v>
@@ -21318,7 +21319,7 @@
       </c>
       <c r="B24" s="15">
         <f ca="1">ModelInput!B37/60*ModelInput!B22</f>
-        <v>4.25</v>
+        <v>3.5155666922186835</v>
       </c>
       <c r="C24" t="s">
         <v>240</v>
@@ -21337,7 +21338,7 @@
       </c>
       <c r="B25" s="15">
         <f ca="1">B24*ModelInput!B36*ModelInput!B17*ModelOutput!B18</f>
-        <v>180.2</v>
+        <v>274.43381832754386</v>
       </c>
       <c r="C25" t="s">
         <v>217</v>
@@ -21356,7 +21357,7 @@
       </c>
       <c r="B26" s="15">
         <f ca="1">B22+B23+B25</f>
-        <v>910.32799999999997</v>
+        <v>410.96181832754388</v>
       </c>
       <c r="C26" t="s">
         <v>217</v>
@@ -21375,7 +21376,7 @@
       </c>
       <c r="B27" s="15">
         <f ca="1">12*ModelInput!B32</f>
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="C27" t="s">
         <v>217</v>
@@ -21394,7 +21395,7 @@
       </c>
       <c r="B28" s="15">
         <f ca="1">B20*(B27+B26)</f>
-        <v>3310.328</v>
+        <v>1910.9618183275438</v>
       </c>
       <c r="C28" t="s">
         <v>217</v>
@@ -21413,7 +21414,7 @@
       </c>
       <c r="B29" s="15">
         <f ca="1">B28*ModelInput!B8</f>
-        <v>23172.295999999998</v>
+        <v>3821.9236366550876</v>
       </c>
       <c r="C29" t="s">
         <v>164</v>
@@ -21432,7 +21433,7 @@
       </c>
       <c r="B30" s="15">
         <f ca="1">B20*ModelInput!B33</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>164</v>
@@ -21460,7 +21461,7 @@
       </c>
       <c r="B32" s="15">
         <f ca="1">B7-B21</f>
-        <v>-41000</v>
+        <v>-13000</v>
       </c>
       <c r="F32">
         <v>29</v>
@@ -21476,7 +21477,7 @@
       </c>
       <c r="B33" s="15">
         <f ca="1">B12-B28</f>
-        <v>7386.3340000000007</v>
+        <v>8785.7001816724569</v>
       </c>
       <c r="F33">
         <v>30</v>
@@ -21492,7 +21493,7 @@
       </c>
       <c r="B34" s="15">
         <f ca="1">B14-B30</f>
-        <v>-2200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -21506,7 +21507,7 @@
       </c>
       <c r="B37" s="15">
         <f ca="1">B7+ModelInput!B8*ModelOutput!B12+ModelOutput!B14</f>
-        <v>150676.63400000002</v>
+        <v>34393.324000000001</v>
       </c>
       <c r="C37" t="s">
         <v>164</v>
@@ -21521,7 +21522,7 @@
       </c>
       <c r="B38" s="15">
         <f ca="1">B21+ModelInput!B8*ModelOutput!B28+ModelOutput!B30</f>
-        <v>142172.296</v>
+        <v>29821.923636655087</v>
       </c>
       <c r="C38" t="s">
         <v>164</v>
@@ -21541,7 +21542,7 @@
       </c>
       <c r="B41" s="19">
         <f ca="1">NPV(ModelInput!B3,G3:G33)</f>
-        <v>168.1787005780028</v>
+        <v>3177.354819072269</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>164</v>
@@ -21558,7 +21559,7 @@
       </c>
       <c r="B44" s="16">
         <f ca="1">NPER(ModelInput!B3,ModelOutput!B33,ModelOutput!B32)</f>
-        <v>6.6630773081481927</v>
+        <v>1.5753915668430523</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
started working on the monthly cost generator
</commit_message>
<xml_diff>
--- a/Excel/AGVUseCaseModel.xlsx
+++ b/Excel/AGVUseCaseModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ew\Documents\GitHub\AGVeval\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9308E65-8788-4CF8-8464-0AC4FA758138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E8D2F-9DED-4C00-A432-FFEF6571C896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{0EF2771D-CFB8-4DE0-9494-6A24E6C64F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <sheet name="MissionModel" sheetId="9" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="286">
   <si>
     <t>Redistribution and use in source and binary forms, with or without modification, are permitted provided that the following conditions are met:</t>
   </si>
@@ -921,6 +920,15 @@
   </si>
   <si>
     <t>Baseline</t>
+  </si>
+  <si>
+    <t>Operating costs</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Autonomous Ground Vehicle</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1025,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1040,8 +1048,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -20898,10 +20905,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3921CD35-E3FB-4076-863C-CDE02BDE2C9B}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20909,6 +20916,7 @@
     <col min="1" max="1" width="50.140625" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -21470,7 +21478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>242</v>
       </c>
@@ -21486,7 +21494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>243</v>
       </c>
@@ -21495,12 +21503,12 @@
         <v>-2200</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>244</v>
       </c>
@@ -21515,7 +21523,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>245</v>
       </c>
@@ -21530,29 +21538,29 @@
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>247</v>
       </c>
-      <c r="B41" s="19">
+      <c r="B41" s="18">
         <f ca="1">NPV(ModelInput!B3,G3:G33)</f>
         <v>168.1787005780028</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>252</v>
       </c>
@@ -21562,6 +21570,2609 @@
       </c>
       <c r="C44" s="2" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F45" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>284</v>
+      </c>
+      <c r="G46" t="s">
+        <v>224</v>
+      </c>
+      <c r="H46" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" s="15">
+        <f ca="1">B7</f>
+        <v>74000</v>
+      </c>
+      <c r="H47" s="15">
+        <f ca="1">B21</f>
+        <v>115000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" s="15">
+        <f ca="1">G47+2*$B$13/12</f>
+        <v>86479.438999999998</v>
+      </c>
+      <c r="H48" s="15">
+        <f ca="1">H47+2*$B$29/12</f>
+        <v>118862.04933333333</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49" s="15">
+        <f t="shared" ref="G49:G112" ca="1" si="0">G48+2*$B$13/12</f>
+        <v>98958.877999999997</v>
+      </c>
+      <c r="H49" s="15">
+        <f t="shared" ref="H49:H112" ca="1" si="1">H48+2*$B$29/12</f>
+        <v>122724.09866666666</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>6</v>
+      </c>
+      <c r="G50" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>111438.317</v>
+      </c>
+      <c r="H50" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>126586.14799999999</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>123917.75599999999</v>
+      </c>
+      <c r="H51" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>130448.19733333332</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>10</v>
+      </c>
+      <c r="G52" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>136397.19500000001</v>
+      </c>
+      <c r="H52" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>134310.24666666664</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>12</v>
+      </c>
+      <c r="G53" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>148876.63400000002</v>
+      </c>
+      <c r="H53" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>138172.29599999997</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>14</v>
+      </c>
+      <c r="G54" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>161356.07300000003</v>
+      </c>
+      <c r="H54" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>142034.3453333333</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>16</v>
+      </c>
+      <c r="G55" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>173835.51200000005</v>
+      </c>
+      <c r="H55" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>145896.39466666663</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>18</v>
+      </c>
+      <c r="G56" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>186314.95100000006</v>
+      </c>
+      <c r="H56" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>149758.44399999996</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>20</v>
+      </c>
+      <c r="G57" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>198794.39000000007</v>
+      </c>
+      <c r="H57" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>153620.49333333329</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>22</v>
+      </c>
+      <c r="G58" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>211273.82900000009</v>
+      </c>
+      <c r="H58" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>157482.54266666662</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>24</v>
+      </c>
+      <c r="G59" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>223753.2680000001</v>
+      </c>
+      <c r="H59" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>161344.59199999995</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>26</v>
+      </c>
+      <c r="G60" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>236232.70700000011</v>
+      </c>
+      <c r="H60" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>165206.64133333327</v>
+      </c>
+    </row>
+    <row r="61" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>28</v>
+      </c>
+      <c r="G61" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>248712.14600000012</v>
+      </c>
+      <c r="H61" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>169068.6906666666</v>
+      </c>
+    </row>
+    <row r="62" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>30</v>
+      </c>
+      <c r="G62" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>261191.58500000014</v>
+      </c>
+      <c r="H62" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>172930.73999999993</v>
+      </c>
+    </row>
+    <row r="63" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>32</v>
+      </c>
+      <c r="G63" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>273671.02400000015</v>
+      </c>
+      <c r="H63" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>176792.78933333326</v>
+      </c>
+    </row>
+    <row r="64" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>34</v>
+      </c>
+      <c r="G64" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>286150.46300000016</v>
+      </c>
+      <c r="H64" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>180654.83866666659</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>36</v>
+      </c>
+      <c r="G65" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>298629.90200000018</v>
+      </c>
+      <c r="H65" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>184516.88799999992</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>38</v>
+      </c>
+      <c r="G66" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>311109.34100000019</v>
+      </c>
+      <c r="H66" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>188378.93733333325</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>40</v>
+      </c>
+      <c r="G67" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>323588.7800000002</v>
+      </c>
+      <c r="H67" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>192240.98666666658</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>42</v>
+      </c>
+      <c r="G68" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>336068.21900000022</v>
+      </c>
+      <c r="H68" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>196103.03599999991</v>
+      </c>
+    </row>
+    <row r="69" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>44</v>
+      </c>
+      <c r="G69" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>348547.65800000023</v>
+      </c>
+      <c r="H69" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>199965.08533333323</v>
+      </c>
+    </row>
+    <row r="70" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>46</v>
+      </c>
+      <c r="G70" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>361027.09700000024</v>
+      </c>
+      <c r="H70" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>203827.13466666656</v>
+      </c>
+    </row>
+    <row r="71" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>48</v>
+      </c>
+      <c r="G71" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>373506.53600000025</v>
+      </c>
+      <c r="H71" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>207689.18399999989</v>
+      </c>
+    </row>
+    <row r="72" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>50</v>
+      </c>
+      <c r="G72" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>385985.97500000027</v>
+      </c>
+      <c r="H72" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>211551.23333333322</v>
+      </c>
+    </row>
+    <row r="73" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>52</v>
+      </c>
+      <c r="G73" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>398465.41400000028</v>
+      </c>
+      <c r="H73" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>215413.28266666655</v>
+      </c>
+    </row>
+    <row r="74" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>54</v>
+      </c>
+      <c r="G74" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>410944.85300000029</v>
+      </c>
+      <c r="H74" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>219275.33199999988</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>56</v>
+      </c>
+      <c r="G75" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>423424.29200000031</v>
+      </c>
+      <c r="H75" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>223137.38133333321</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>58</v>
+      </c>
+      <c r="G76" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>435903.73100000032</v>
+      </c>
+      <c r="H76" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>226999.43066666654</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>60</v>
+      </c>
+      <c r="G77" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>448383.17000000033</v>
+      </c>
+      <c r="H77" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>230861.47999999986</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>62</v>
+      </c>
+      <c r="G78" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>460862.60900000035</v>
+      </c>
+      <c r="H78" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>234723.52933333319</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>64</v>
+      </c>
+      <c r="G79" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>473342.04800000036</v>
+      </c>
+      <c r="H79" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>238585.57866666652</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>66</v>
+      </c>
+      <c r="G80" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>485821.48700000037</v>
+      </c>
+      <c r="H80" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>242447.62799999985</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>68</v>
+      </c>
+      <c r="G81" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>498300.92600000039</v>
+      </c>
+      <c r="H81" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>246309.67733333318</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>70</v>
+      </c>
+      <c r="G82" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>510780.3650000004</v>
+      </c>
+      <c r="H82" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>250171.72666666651</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>72</v>
+      </c>
+      <c r="G83" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>523259.80400000041</v>
+      </c>
+      <c r="H83" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>254033.77599999984</v>
+      </c>
+    </row>
+    <row r="84" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>74</v>
+      </c>
+      <c r="G84" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>535739.24300000037</v>
+      </c>
+      <c r="H84" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>257895.82533333317</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>76</v>
+      </c>
+      <c r="G85" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>548218.68200000038</v>
+      </c>
+      <c r="H85" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>261757.8746666665</v>
+      </c>
+    </row>
+    <row r="86" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>78</v>
+      </c>
+      <c r="G86" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>560698.12100000039</v>
+      </c>
+      <c r="H86" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>265619.92399999982</v>
+      </c>
+    </row>
+    <row r="87" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>80</v>
+      </c>
+      <c r="G87" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>573177.56000000041</v>
+      </c>
+      <c r="H87" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>269481.97333333315</v>
+      </c>
+    </row>
+    <row r="88" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>82</v>
+      </c>
+      <c r="G88" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>585656.99900000042</v>
+      </c>
+      <c r="H88" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>273344.02266666648</v>
+      </c>
+    </row>
+    <row r="89" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>84</v>
+      </c>
+      <c r="G89" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>598136.43800000043</v>
+      </c>
+      <c r="H89" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>277206.07199999981</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>86</v>
+      </c>
+      <c r="G90" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>610615.87700000044</v>
+      </c>
+      <c r="H90" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>281068.12133333314</v>
+      </c>
+    </row>
+    <row r="91" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>88</v>
+      </c>
+      <c r="G91" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>623095.31600000046</v>
+      </c>
+      <c r="H91" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>284930.17066666647</v>
+      </c>
+    </row>
+    <row r="92" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>90</v>
+      </c>
+      <c r="G92" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>635574.75500000047</v>
+      </c>
+      <c r="H92" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>288792.2199999998</v>
+      </c>
+    </row>
+    <row r="93" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>92</v>
+      </c>
+      <c r="G93" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>648054.19400000048</v>
+      </c>
+      <c r="H93" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>292654.26933333313</v>
+      </c>
+    </row>
+    <row r="94" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>94</v>
+      </c>
+      <c r="G94" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>660533.6330000005</v>
+      </c>
+      <c r="H94" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>296516.31866666646</v>
+      </c>
+    </row>
+    <row r="95" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>96</v>
+      </c>
+      <c r="G95" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>673013.07200000051</v>
+      </c>
+      <c r="H95" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>300378.36799999978</v>
+      </c>
+    </row>
+    <row r="96" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>98</v>
+      </c>
+      <c r="G96" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>685492.51100000052</v>
+      </c>
+      <c r="H96" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>304240.41733333311</v>
+      </c>
+    </row>
+    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>100</v>
+      </c>
+      <c r="G97" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>697971.95000000054</v>
+      </c>
+      <c r="H97" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>308102.46666666644</v>
+      </c>
+    </row>
+    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>102</v>
+      </c>
+      <c r="G98" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>710451.38900000055</v>
+      </c>
+      <c r="H98" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>311964.51599999977</v>
+      </c>
+    </row>
+    <row r="99" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>104</v>
+      </c>
+      <c r="G99" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>722930.82800000056</v>
+      </c>
+      <c r="H99" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>315826.5653333331</v>
+      </c>
+    </row>
+    <row r="100" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>106</v>
+      </c>
+      <c r="G100" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>735410.26700000057</v>
+      </c>
+      <c r="H100" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>319688.61466666643</v>
+      </c>
+    </row>
+    <row r="101" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <v>108</v>
+      </c>
+      <c r="G101" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>747889.70600000059</v>
+      </c>
+      <c r="H101" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>323550.66399999976</v>
+      </c>
+    </row>
+    <row r="102" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <v>110</v>
+      </c>
+      <c r="G102" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>760369.1450000006</v>
+      </c>
+      <c r="H102" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>327412.71333333309</v>
+      </c>
+    </row>
+    <row r="103" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <v>112</v>
+      </c>
+      <c r="G103" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>772848.58400000061</v>
+      </c>
+      <c r="H103" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>331274.76266666641</v>
+      </c>
+    </row>
+    <row r="104" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <v>114</v>
+      </c>
+      <c r="G104" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>785328.02300000063</v>
+      </c>
+      <c r="H104" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>335136.81199999974</v>
+      </c>
+    </row>
+    <row r="105" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <v>116</v>
+      </c>
+      <c r="G105" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>797807.46200000064</v>
+      </c>
+      <c r="H105" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>338998.86133333307</v>
+      </c>
+    </row>
+    <row r="106" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <v>118</v>
+      </c>
+      <c r="G106" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>810286.90100000065</v>
+      </c>
+      <c r="H106" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>342860.9106666664</v>
+      </c>
+    </row>
+    <row r="107" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <v>120</v>
+      </c>
+      <c r="G107" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>822766.34000000067</v>
+      </c>
+      <c r="H107" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>346722.95999999973</v>
+      </c>
+    </row>
+    <row r="108" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <v>122</v>
+      </c>
+      <c r="G108" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>835245.77900000068</v>
+      </c>
+      <c r="H108" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>350585.00933333306</v>
+      </c>
+    </row>
+    <row r="109" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <v>124</v>
+      </c>
+      <c r="G109" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>847725.21800000069</v>
+      </c>
+      <c r="H109" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>354447.05866666639</v>
+      </c>
+    </row>
+    <row r="110" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <v>126</v>
+      </c>
+      <c r="G110" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>860204.65700000071</v>
+      </c>
+      <c r="H110" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>358309.10799999972</v>
+      </c>
+    </row>
+    <row r="111" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <v>128</v>
+      </c>
+      <c r="G111" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>872684.09600000072</v>
+      </c>
+      <c r="H111" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>362171.15733333305</v>
+      </c>
+    </row>
+    <row r="112" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <v>130</v>
+      </c>
+      <c r="G112" s="15">
+        <f t="shared" ca="1" si="0"/>
+        <v>885163.53500000073</v>
+      </c>
+      <c r="H112" s="15">
+        <f t="shared" ca="1" si="1"/>
+        <v>366033.20666666637</v>
+      </c>
+    </row>
+    <row r="113" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <v>132</v>
+      </c>
+      <c r="G113" s="15">
+        <f t="shared" ref="G113:G176" ca="1" si="2">G112+2*$B$13/12</f>
+        <v>897642.97400000074</v>
+      </c>
+      <c r="H113" s="15">
+        <f t="shared" ref="H113:H176" ca="1" si="3">H112+2*$B$29/12</f>
+        <v>369895.2559999997</v>
+      </c>
+    </row>
+    <row r="114" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <v>134</v>
+      </c>
+      <c r="G114" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>910122.41300000076</v>
+      </c>
+      <c r="H114" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>373757.30533333303</v>
+      </c>
+    </row>
+    <row r="115" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <v>136</v>
+      </c>
+      <c r="G115" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>922601.85200000077</v>
+      </c>
+      <c r="H115" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>377619.35466666636</v>
+      </c>
+    </row>
+    <row r="116" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <v>138</v>
+      </c>
+      <c r="G116" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>935081.29100000078</v>
+      </c>
+      <c r="H116" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>381481.40399999969</v>
+      </c>
+    </row>
+    <row r="117" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <v>140</v>
+      </c>
+      <c r="G117" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>947560.7300000008</v>
+      </c>
+      <c r="H117" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>385343.45333333302</v>
+      </c>
+    </row>
+    <row r="118" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <v>142</v>
+      </c>
+      <c r="G118" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>960040.16900000081</v>
+      </c>
+      <c r="H118" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>389205.50266666635</v>
+      </c>
+    </row>
+    <row r="119" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <v>144</v>
+      </c>
+      <c r="G119" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>972519.60800000082</v>
+      </c>
+      <c r="H119" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>393067.55199999968</v>
+      </c>
+    </row>
+    <row r="120" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <v>146</v>
+      </c>
+      <c r="G120" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>984999.04700000084</v>
+      </c>
+      <c r="H120" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>396929.601333333</v>
+      </c>
+    </row>
+    <row r="121" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <v>148</v>
+      </c>
+      <c r="G121" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>997478.48600000085</v>
+      </c>
+      <c r="H121" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>400791.65066666633</v>
+      </c>
+    </row>
+    <row r="122" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <v>150</v>
+      </c>
+      <c r="G122" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1009957.9250000009</v>
+      </c>
+      <c r="H122" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>404653.69999999966</v>
+      </c>
+    </row>
+    <row r="123" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <v>152</v>
+      </c>
+      <c r="G123" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1022437.3640000009</v>
+      </c>
+      <c r="H123" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>408515.74933333299</v>
+      </c>
+    </row>
+    <row r="124" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <v>154</v>
+      </c>
+      <c r="G124" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1034916.8030000009</v>
+      </c>
+      <c r="H124" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>412377.79866666632</v>
+      </c>
+    </row>
+    <row r="125" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>156</v>
+      </c>
+      <c r="G125" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1047396.2420000009</v>
+      </c>
+      <c r="H125" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>416239.84799999965</v>
+      </c>
+    </row>
+    <row r="126" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <v>158</v>
+      </c>
+      <c r="G126" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1059875.6810000008</v>
+      </c>
+      <c r="H126" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>420101.89733333298</v>
+      </c>
+    </row>
+    <row r="127" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <v>160</v>
+      </c>
+      <c r="G127" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1072355.1200000008</v>
+      </c>
+      <c r="H127" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>423963.94666666631</v>
+      </c>
+    </row>
+    <row r="128" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <v>162</v>
+      </c>
+      <c r="G128" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1084834.5590000008</v>
+      </c>
+      <c r="H128" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>427825.99599999964</v>
+      </c>
+    </row>
+    <row r="129" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <v>164</v>
+      </c>
+      <c r="G129" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1097313.9980000008</v>
+      </c>
+      <c r="H129" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>431688.04533333296</v>
+      </c>
+    </row>
+    <row r="130" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <v>166</v>
+      </c>
+      <c r="G130" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1109793.4370000008</v>
+      </c>
+      <c r="H130" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>435550.09466666629</v>
+      </c>
+    </row>
+    <row r="131" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F131">
+        <v>168</v>
+      </c>
+      <c r="G131" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1122272.8760000009</v>
+      </c>
+      <c r="H131" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>439412.14399999962</v>
+      </c>
+    </row>
+    <row r="132" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F132">
+        <v>170</v>
+      </c>
+      <c r="G132" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1134752.3150000009</v>
+      </c>
+      <c r="H132" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>443274.19333333295</v>
+      </c>
+    </row>
+    <row r="133" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F133">
+        <v>172</v>
+      </c>
+      <c r="G133" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1147231.7540000009</v>
+      </c>
+      <c r="H133" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>447136.24266666628</v>
+      </c>
+    </row>
+    <row r="134" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F134">
+        <v>174</v>
+      </c>
+      <c r="G134" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1159711.1930000009</v>
+      </c>
+      <c r="H134" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>450998.29199999961</v>
+      </c>
+    </row>
+    <row r="135" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F135">
+        <v>176</v>
+      </c>
+      <c r="G135" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1172190.6320000009</v>
+      </c>
+      <c r="H135" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>454860.34133333294</v>
+      </c>
+    </row>
+    <row r="136" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F136">
+        <v>178</v>
+      </c>
+      <c r="G136" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1184670.0710000009</v>
+      </c>
+      <c r="H136" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>458722.39066666627</v>
+      </c>
+    </row>
+    <row r="137" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F137">
+        <v>180</v>
+      </c>
+      <c r="G137" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1197149.5100000009</v>
+      </c>
+      <c r="H137" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>462584.43999999959</v>
+      </c>
+    </row>
+    <row r="138" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F138">
+        <v>182</v>
+      </c>
+      <c r="G138" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1209628.949000001</v>
+      </c>
+      <c r="H138" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>466446.48933333292</v>
+      </c>
+    </row>
+    <row r="139" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F139">
+        <v>184</v>
+      </c>
+      <c r="G139" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1222108.388000001</v>
+      </c>
+      <c r="H139" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>470308.53866666625</v>
+      </c>
+    </row>
+    <row r="140" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F140">
+        <v>186</v>
+      </c>
+      <c r="G140" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1234587.827000001</v>
+      </c>
+      <c r="H140" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>474170.58799999958</v>
+      </c>
+    </row>
+    <row r="141" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <v>188</v>
+      </c>
+      <c r="G141" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1247067.266000001</v>
+      </c>
+      <c r="H141" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>478032.63733333291</v>
+      </c>
+    </row>
+    <row r="142" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F142">
+        <v>190</v>
+      </c>
+      <c r="G142" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1259546.705000001</v>
+      </c>
+      <c r="H142" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>481894.68666666624</v>
+      </c>
+    </row>
+    <row r="143" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F143">
+        <v>192</v>
+      </c>
+      <c r="G143" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1272026.144000001</v>
+      </c>
+      <c r="H143" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>485756.73599999957</v>
+      </c>
+    </row>
+    <row r="144" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F144">
+        <v>194</v>
+      </c>
+      <c r="G144" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1284505.583000001</v>
+      </c>
+      <c r="H144" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>489618.7853333329</v>
+      </c>
+    </row>
+    <row r="145" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F145">
+        <v>196</v>
+      </c>
+      <c r="G145" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1296985.022000001</v>
+      </c>
+      <c r="H145" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>493480.83466666623</v>
+      </c>
+    </row>
+    <row r="146" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F146">
+        <v>198</v>
+      </c>
+      <c r="G146" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1309464.4610000011</v>
+      </c>
+      <c r="H146" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>497342.88399999955</v>
+      </c>
+    </row>
+    <row r="147" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F147">
+        <v>200</v>
+      </c>
+      <c r="G147" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1321943.9000000011</v>
+      </c>
+      <c r="H147" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>501204.93333333288</v>
+      </c>
+    </row>
+    <row r="148" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F148">
+        <v>202</v>
+      </c>
+      <c r="G148" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1334423.3390000011</v>
+      </c>
+      <c r="H148" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>505066.98266666621</v>
+      </c>
+    </row>
+    <row r="149" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F149">
+        <v>204</v>
+      </c>
+      <c r="G149" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1346902.7780000011</v>
+      </c>
+      <c r="H149" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>508929.03199999954</v>
+      </c>
+    </row>
+    <row r="150" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F150">
+        <v>206</v>
+      </c>
+      <c r="G150" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1359382.2170000011</v>
+      </c>
+      <c r="H150" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>512791.08133333287</v>
+      </c>
+    </row>
+    <row r="151" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F151">
+        <v>208</v>
+      </c>
+      <c r="G151" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1371861.6560000011</v>
+      </c>
+      <c r="H151" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>516653.1306666662</v>
+      </c>
+    </row>
+    <row r="152" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F152">
+        <v>210</v>
+      </c>
+      <c r="G152" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1384341.0950000011</v>
+      </c>
+      <c r="H152" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>520515.17999999953</v>
+      </c>
+    </row>
+    <row r="153" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F153">
+        <v>212</v>
+      </c>
+      <c r="G153" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1396820.5340000011</v>
+      </c>
+      <c r="H153" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>524377.22933333286</v>
+      </c>
+    </row>
+    <row r="154" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F154">
+        <v>214</v>
+      </c>
+      <c r="G154" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1409299.9730000012</v>
+      </c>
+      <c r="H154" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>528239.27866666624</v>
+      </c>
+    </row>
+    <row r="155" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F155">
+        <v>216</v>
+      </c>
+      <c r="G155" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1421779.4120000012</v>
+      </c>
+      <c r="H155" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>532101.32799999963</v>
+      </c>
+    </row>
+    <row r="156" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <v>218</v>
+      </c>
+      <c r="G156" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1434258.8510000012</v>
+      </c>
+      <c r="H156" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>535963.37733333302</v>
+      </c>
+    </row>
+    <row r="157" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <v>220</v>
+      </c>
+      <c r="G157" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1446738.2900000012</v>
+      </c>
+      <c r="H157" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>539825.4266666664</v>
+      </c>
+    </row>
+    <row r="158" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <v>222</v>
+      </c>
+      <c r="G158" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1459217.7290000012</v>
+      </c>
+      <c r="H158" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>543687.47599999979</v>
+      </c>
+    </row>
+    <row r="159" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <v>224</v>
+      </c>
+      <c r="G159" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1471697.1680000012</v>
+      </c>
+      <c r="H159" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>547549.52533333318</v>
+      </c>
+    </row>
+    <row r="160" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <v>226</v>
+      </c>
+      <c r="G160" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1484176.6070000012</v>
+      </c>
+      <c r="H160" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>551411.57466666657</v>
+      </c>
+    </row>
+    <row r="161" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <v>228</v>
+      </c>
+      <c r="G161" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1496656.0460000013</v>
+      </c>
+      <c r="H161" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>555273.62399999995</v>
+      </c>
+    </row>
+    <row r="162" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <v>230</v>
+      </c>
+      <c r="G162" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1509135.4850000013</v>
+      </c>
+      <c r="H162" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>559135.67333333334</v>
+      </c>
+    </row>
+    <row r="163" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <v>232</v>
+      </c>
+      <c r="G163" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1521614.9240000013</v>
+      </c>
+      <c r="H163" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>562997.72266666673</v>
+      </c>
+    </row>
+    <row r="164" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <v>234</v>
+      </c>
+      <c r="G164" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1534094.3630000013</v>
+      </c>
+      <c r="H164" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>566859.77200000011</v>
+      </c>
+    </row>
+    <row r="165" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <v>236</v>
+      </c>
+      <c r="G165" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1546573.8020000013</v>
+      </c>
+      <c r="H165" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>570721.8213333335</v>
+      </c>
+    </row>
+    <row r="166" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <v>238</v>
+      </c>
+      <c r="G166" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1559053.2410000013</v>
+      </c>
+      <c r="H166" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>574583.87066666689</v>
+      </c>
+    </row>
+    <row r="167" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F167">
+        <v>240</v>
+      </c>
+      <c r="G167" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1571532.6800000013</v>
+      </c>
+      <c r="H167" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>578445.92000000027</v>
+      </c>
+    </row>
+    <row r="168" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <v>242</v>
+      </c>
+      <c r="G168" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1584012.1190000013</v>
+      </c>
+      <c r="H168" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>582307.96933333366</v>
+      </c>
+    </row>
+    <row r="169" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <v>244</v>
+      </c>
+      <c r="G169" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1596491.5580000014</v>
+      </c>
+      <c r="H169" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>586170.01866666705</v>
+      </c>
+    </row>
+    <row r="170" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <v>246</v>
+      </c>
+      <c r="G170" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1608970.9970000014</v>
+      </c>
+      <c r="H170" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>590032.06800000044</v>
+      </c>
+    </row>
+    <row r="171" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <v>248</v>
+      </c>
+      <c r="G171" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1621450.4360000014</v>
+      </c>
+      <c r="H171" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>593894.11733333382</v>
+      </c>
+    </row>
+    <row r="172" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <v>250</v>
+      </c>
+      <c r="G172" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1633929.8750000014</v>
+      </c>
+      <c r="H172" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>597756.16666666721</v>
+      </c>
+    </row>
+    <row r="173" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <v>252</v>
+      </c>
+      <c r="G173" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1646409.3140000014</v>
+      </c>
+      <c r="H173" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>601618.2160000006</v>
+      </c>
+    </row>
+    <row r="174" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <v>254</v>
+      </c>
+      <c r="G174" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1658888.7530000014</v>
+      </c>
+      <c r="H174" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>605480.26533333398</v>
+      </c>
+    </row>
+    <row r="175" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F175">
+        <v>256</v>
+      </c>
+      <c r="G175" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1671368.1920000014</v>
+      </c>
+      <c r="H175" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>609342.31466666737</v>
+      </c>
+    </row>
+    <row r="176" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F176">
+        <v>258</v>
+      </c>
+      <c r="G176" s="15">
+        <f t="shared" ca="1" si="2"/>
+        <v>1683847.6310000014</v>
+      </c>
+      <c r="H176" s="15">
+        <f t="shared" ca="1" si="3"/>
+        <v>613204.36400000076</v>
+      </c>
+    </row>
+    <row r="177" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F177">
+        <v>260</v>
+      </c>
+      <c r="G177" s="15">
+        <f t="shared" ref="G177:G240" ca="1" si="4">G176+2*$B$13/12</f>
+        <v>1696327.0700000015</v>
+      </c>
+      <c r="H177" s="15">
+        <f t="shared" ref="H177:H240" ca="1" si="5">H176+2*$B$29/12</f>
+        <v>617066.41333333415</v>
+      </c>
+    </row>
+    <row r="178" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F178">
+        <v>262</v>
+      </c>
+      <c r="G178" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1708806.5090000015</v>
+      </c>
+      <c r="H178" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>620928.46266666753</v>
+      </c>
+    </row>
+    <row r="179" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F179">
+        <v>264</v>
+      </c>
+      <c r="G179" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1721285.9480000015</v>
+      </c>
+      <c r="H179" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>624790.51200000092</v>
+      </c>
+    </row>
+    <row r="180" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F180">
+        <v>266</v>
+      </c>
+      <c r="G180" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1733765.3870000015</v>
+      </c>
+      <c r="H180" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>628652.56133333431</v>
+      </c>
+    </row>
+    <row r="181" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F181">
+        <v>268</v>
+      </c>
+      <c r="G181" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1746244.8260000015</v>
+      </c>
+      <c r="H181" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>632514.61066666769</v>
+      </c>
+    </row>
+    <row r="182" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F182">
+        <v>270</v>
+      </c>
+      <c r="G182" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1758724.2650000015</v>
+      </c>
+      <c r="H182" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>636376.66000000108</v>
+      </c>
+    </row>
+    <row r="183" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F183">
+        <v>272</v>
+      </c>
+      <c r="G183" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1771203.7040000015</v>
+      </c>
+      <c r="H183" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>640238.70933333447</v>
+      </c>
+    </row>
+    <row r="184" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F184">
+        <v>274</v>
+      </c>
+      <c r="G184" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1783683.1430000016</v>
+      </c>
+      <c r="H184" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>644100.75866666785</v>
+      </c>
+    </row>
+    <row r="185" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F185">
+        <v>276</v>
+      </c>
+      <c r="G185" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1796162.5820000016</v>
+      </c>
+      <c r="H185" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>647962.80800000124</v>
+      </c>
+    </row>
+    <row r="186" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F186">
+        <v>278</v>
+      </c>
+      <c r="G186" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1808642.0210000016</v>
+      </c>
+      <c r="H186" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>651824.85733333463</v>
+      </c>
+    </row>
+    <row r="187" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F187">
+        <v>280</v>
+      </c>
+      <c r="G187" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1821121.4600000016</v>
+      </c>
+      <c r="H187" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>655686.90666666802</v>
+      </c>
+    </row>
+    <row r="188" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F188">
+        <v>282</v>
+      </c>
+      <c r="G188" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1833600.8990000016</v>
+      </c>
+      <c r="H188" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>659548.9560000014</v>
+      </c>
+    </row>
+    <row r="189" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F189">
+        <v>284</v>
+      </c>
+      <c r="G189" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1846080.3380000016</v>
+      </c>
+      <c r="H189" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>663411.00533333479</v>
+      </c>
+    </row>
+    <row r="190" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F190">
+        <v>286</v>
+      </c>
+      <c r="G190" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1858559.7770000016</v>
+      </c>
+      <c r="H190" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>667273.05466666818</v>
+      </c>
+    </row>
+    <row r="191" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F191">
+        <v>288</v>
+      </c>
+      <c r="G191" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1871039.2160000016</v>
+      </c>
+      <c r="H191" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>671135.10400000156</v>
+      </c>
+    </row>
+    <row r="192" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F192">
+        <v>290</v>
+      </c>
+      <c r="G192" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1883518.6550000017</v>
+      </c>
+      <c r="H192" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>674997.15333333495</v>
+      </c>
+    </row>
+    <row r="193" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F193">
+        <v>292</v>
+      </c>
+      <c r="G193" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1895998.0940000017</v>
+      </c>
+      <c r="H193" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>678859.20266666834</v>
+      </c>
+    </row>
+    <row r="194" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F194">
+        <v>294</v>
+      </c>
+      <c r="G194" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1908477.5330000017</v>
+      </c>
+      <c r="H194" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>682721.25200000172</v>
+      </c>
+    </row>
+    <row r="195" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F195">
+        <v>296</v>
+      </c>
+      <c r="G195" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1920956.9720000017</v>
+      </c>
+      <c r="H195" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>686583.30133333511</v>
+      </c>
+    </row>
+    <row r="196" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F196">
+        <v>298</v>
+      </c>
+      <c r="G196" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1933436.4110000017</v>
+      </c>
+      <c r="H196" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>690445.3506666685</v>
+      </c>
+    </row>
+    <row r="197" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F197">
+        <v>300</v>
+      </c>
+      <c r="G197" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1945915.8500000017</v>
+      </c>
+      <c r="H197" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>694307.40000000189</v>
+      </c>
+    </row>
+    <row r="198" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F198">
+        <v>302</v>
+      </c>
+      <c r="G198" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1958395.2890000017</v>
+      </c>
+      <c r="H198" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>698169.44933333527</v>
+      </c>
+    </row>
+    <row r="199" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F199">
+        <v>304</v>
+      </c>
+      <c r="G199" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1970874.7280000017</v>
+      </c>
+      <c r="H199" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>702031.49866666866</v>
+      </c>
+    </row>
+    <row r="200" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F200">
+        <v>306</v>
+      </c>
+      <c r="G200" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1983354.1670000018</v>
+      </c>
+      <c r="H200" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>705893.54800000205</v>
+      </c>
+    </row>
+    <row r="201" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F201">
+        <v>308</v>
+      </c>
+      <c r="G201" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>1995833.6060000018</v>
+      </c>
+      <c r="H201" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>709755.59733333543</v>
+      </c>
+    </row>
+    <row r="202" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F202">
+        <v>310</v>
+      </c>
+      <c r="G202" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2008313.0450000018</v>
+      </c>
+      <c r="H202" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>713617.64666666882</v>
+      </c>
+    </row>
+    <row r="203" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F203">
+        <v>312</v>
+      </c>
+      <c r="G203" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2020792.4840000018</v>
+      </c>
+      <c r="H203" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>717479.69600000221</v>
+      </c>
+    </row>
+    <row r="204" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F204">
+        <v>314</v>
+      </c>
+      <c r="G204" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2033271.9230000018</v>
+      </c>
+      <c r="H204" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>721341.7453333356</v>
+      </c>
+    </row>
+    <row r="205" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F205">
+        <v>316</v>
+      </c>
+      <c r="G205" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2045751.3620000018</v>
+      </c>
+      <c r="H205" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>725203.79466666898</v>
+      </c>
+    </row>
+    <row r="206" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F206">
+        <v>318</v>
+      </c>
+      <c r="G206" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2058230.8010000018</v>
+      </c>
+      <c r="H206" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>729065.84400000237</v>
+      </c>
+    </row>
+    <row r="207" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F207">
+        <v>320</v>
+      </c>
+      <c r="G207" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2070710.2400000019</v>
+      </c>
+      <c r="H207" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>732927.89333333576</v>
+      </c>
+    </row>
+    <row r="208" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F208">
+        <v>322</v>
+      </c>
+      <c r="G208" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2083189.6790000019</v>
+      </c>
+      <c r="H208" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>736789.94266666914</v>
+      </c>
+    </row>
+    <row r="209" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F209">
+        <v>324</v>
+      </c>
+      <c r="G209" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2095669.1180000019</v>
+      </c>
+      <c r="H209" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>740651.99200000253</v>
+      </c>
+    </row>
+    <row r="210" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F210">
+        <v>326</v>
+      </c>
+      <c r="G210" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2108148.5570000019</v>
+      </c>
+      <c r="H210" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>744514.04133333592</v>
+      </c>
+    </row>
+    <row r="211" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F211">
+        <v>328</v>
+      </c>
+      <c r="G211" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2120627.9960000017</v>
+      </c>
+      <c r="H211" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>748376.0906666693</v>
+      </c>
+    </row>
+    <row r="212" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F212">
+        <v>330</v>
+      </c>
+      <c r="G212" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2133107.4350000015</v>
+      </c>
+      <c r="H212" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>752238.14000000269</v>
+      </c>
+    </row>
+    <row r="213" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F213">
+        <v>332</v>
+      </c>
+      <c r="G213" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2145586.8740000012</v>
+      </c>
+      <c r="H213" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>756100.18933333608</v>
+      </c>
+    </row>
+    <row r="214" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F214">
+        <v>334</v>
+      </c>
+      <c r="G214" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2158066.313000001</v>
+      </c>
+      <c r="H214" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>759962.23866666947</v>
+      </c>
+    </row>
+    <row r="215" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F215">
+        <v>336</v>
+      </c>
+      <c r="G215" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2170545.7520000008</v>
+      </c>
+      <c r="H215" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>763824.28800000285</v>
+      </c>
+    </row>
+    <row r="216" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F216">
+        <v>338</v>
+      </c>
+      <c r="G216" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2183025.1910000006</v>
+      </c>
+      <c r="H216" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>767686.33733333624</v>
+      </c>
+    </row>
+    <row r="217" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F217">
+        <v>340</v>
+      </c>
+      <c r="G217" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2195504.6300000004</v>
+      </c>
+      <c r="H217" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>771548.38666666963</v>
+      </c>
+    </row>
+    <row r="218" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F218">
+        <v>342</v>
+      </c>
+      <c r="G218" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2207984.0690000001</v>
+      </c>
+      <c r="H218" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>775410.43600000301</v>
+      </c>
+    </row>
+    <row r="219" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F219">
+        <v>344</v>
+      </c>
+      <c r="G219" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2220463.5079999999</v>
+      </c>
+      <c r="H219" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>779272.4853333364</v>
+      </c>
+    </row>
+    <row r="220" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F220">
+        <v>346</v>
+      </c>
+      <c r="G220" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2232942.9469999997</v>
+      </c>
+      <c r="H220" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>783134.53466666979</v>
+      </c>
+    </row>
+    <row r="221" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F221">
+        <v>348</v>
+      </c>
+      <c r="G221" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2245422.3859999995</v>
+      </c>
+      <c r="H221" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>786996.58400000317</v>
+      </c>
+    </row>
+    <row r="222" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F222">
+        <v>350</v>
+      </c>
+      <c r="G222" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2257901.8249999993</v>
+      </c>
+      <c r="H222" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>790858.63333333656</v>
+      </c>
+    </row>
+    <row r="223" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F223">
+        <v>352</v>
+      </c>
+      <c r="G223" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2270381.263999999</v>
+      </c>
+      <c r="H223" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>794720.68266666995</v>
+      </c>
+    </row>
+    <row r="224" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F224">
+        <v>354</v>
+      </c>
+      <c r="G224" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2282860.7029999988</v>
+      </c>
+      <c r="H224" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>798582.73200000334</v>
+      </c>
+    </row>
+    <row r="225" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F225">
+        <v>356</v>
+      </c>
+      <c r="G225" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2295340.1419999986</v>
+      </c>
+      <c r="H225" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>802444.78133333672</v>
+      </c>
+    </row>
+    <row r="226" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F226">
+        <v>358</v>
+      </c>
+      <c r="G226" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2307819.5809999984</v>
+      </c>
+      <c r="H226" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>806306.83066667011</v>
+      </c>
+    </row>
+    <row r="227" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F227">
+        <v>360</v>
+      </c>
+      <c r="G227" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2320299.0199999982</v>
+      </c>
+      <c r="H227" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>810168.8800000035</v>
+      </c>
+    </row>
+    <row r="228" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F228">
+        <v>362</v>
+      </c>
+      <c r="G228" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2332778.4589999979</v>
+      </c>
+      <c r="H228" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>814030.92933333688</v>
+      </c>
+    </row>
+    <row r="229" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F229">
+        <v>364</v>
+      </c>
+      <c r="G229" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2345257.8979999977</v>
+      </c>
+      <c r="H229" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>817892.97866667027</v>
+      </c>
+    </row>
+    <row r="230" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F230">
+        <v>366</v>
+      </c>
+      <c r="G230" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2357737.3369999975</v>
+      </c>
+      <c r="H230" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>821755.02800000366</v>
+      </c>
+    </row>
+    <row r="231" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F231">
+        <v>368</v>
+      </c>
+      <c r="G231" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2370216.7759999973</v>
+      </c>
+      <c r="H231" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>825617.07733333705</v>
+      </c>
+    </row>
+    <row r="232" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F232">
+        <v>370</v>
+      </c>
+      <c r="G232" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2382696.2149999971</v>
+      </c>
+      <c r="H232" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>829479.12666667043</v>
+      </c>
+    </row>
+    <row r="233" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F233">
+        <v>372</v>
+      </c>
+      <c r="G233" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2395175.6539999968</v>
+      </c>
+      <c r="H233" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>833341.17600000382</v>
+      </c>
+    </row>
+    <row r="234" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F234">
+        <v>374</v>
+      </c>
+      <c r="G234" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2407655.0929999966</v>
+      </c>
+      <c r="H234" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>837203.22533333721</v>
+      </c>
+    </row>
+    <row r="235" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F235">
+        <v>376</v>
+      </c>
+      <c r="G235" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2420134.5319999964</v>
+      </c>
+      <c r="H235" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>841065.27466667059</v>
+      </c>
+    </row>
+    <row r="236" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F236">
+        <v>378</v>
+      </c>
+      <c r="G236" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2432613.9709999962</v>
+      </c>
+      <c r="H236" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>844927.32400000398</v>
+      </c>
+    </row>
+    <row r="237" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F237">
+        <v>380</v>
+      </c>
+      <c r="G237" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2445093.409999996</v>
+      </c>
+      <c r="H237" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>848789.37333333737</v>
+      </c>
+    </row>
+    <row r="238" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F238">
+        <v>382</v>
+      </c>
+      <c r="G238" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2457572.8489999957</v>
+      </c>
+      <c r="H238" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>852651.42266667075</v>
+      </c>
+    </row>
+    <row r="239" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F239">
+        <v>384</v>
+      </c>
+      <c r="G239" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2470052.2879999955</v>
+      </c>
+      <c r="H239" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>856513.47200000414</v>
+      </c>
+    </row>
+    <row r="240" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F240">
+        <v>386</v>
+      </c>
+      <c r="G240" s="15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2482531.7269999953</v>
+      </c>
+      <c r="H240" s="15">
+        <f t="shared" ca="1" si="5"/>
+        <v>860375.52133333753</v>
+      </c>
+    </row>
+    <row r="241" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F241">
+        <v>388</v>
+      </c>
+      <c r="G241" s="15">
+        <f t="shared" ref="G241:G245" ca="1" si="6">G240+2*$B$13/12</f>
+        <v>2495011.1659999951</v>
+      </c>
+      <c r="H241" s="15">
+        <f t="shared" ref="H241:H245" ca="1" si="7">H240+2*$B$29/12</f>
+        <v>864237.57066667092</v>
+      </c>
+    </row>
+    <row r="242" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F242">
+        <v>390</v>
+      </c>
+      <c r="G242" s="15">
+        <f t="shared" ca="1" si="6"/>
+        <v>2507490.6049999949</v>
+      </c>
+      <c r="H242" s="15">
+        <f t="shared" ca="1" si="7"/>
+        <v>868099.6200000043</v>
+      </c>
+    </row>
+    <row r="243" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F243">
+        <v>392</v>
+      </c>
+      <c r="G243" s="15">
+        <f t="shared" ca="1" si="6"/>
+        <v>2519970.0439999946</v>
+      </c>
+      <c r="H243" s="15">
+        <f t="shared" ca="1" si="7"/>
+        <v>871961.66933333769</v>
+      </c>
+    </row>
+    <row r="244" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F244">
+        <v>394</v>
+      </c>
+      <c r="G244" s="15">
+        <f t="shared" ca="1" si="6"/>
+        <v>2532449.4829999944</v>
+      </c>
+      <c r="H244" s="15">
+        <f t="shared" ca="1" si="7"/>
+        <v>875823.71866667108</v>
+      </c>
+    </row>
+    <row r="245" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F245">
+        <v>396</v>
+      </c>
+      <c r="G245" s="15">
+        <f t="shared" ca="1" si="6"/>
+        <v>2544928.9219999942</v>
+      </c>
+      <c r="H245" s="15">
+        <f t="shared" ca="1" si="7"/>
+        <v>879685.76800000446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>